<commit_message>
updated correction code & cot code
</commit_message>
<xml_diff>
--- a/visualizations/join_results.xlsx
+++ b/visualizations/join_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/visualizations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1B3EA3-31E5-BA43-B694-632654889457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A735C93B-EF65-EF46-8D7F-CDB31A6B868F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="4880" windowWidth="38400" windowHeight="21600" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="4880" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="heuristics" sheetId="10" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="61">
   <si>
     <t>4o-mini</t>
   </si>
@@ -210,13 +210,22 @@
     <t>llama3 (8b)</t>
   </si>
   <si>
-    <t>Zero-Shot (CoT)</t>
-  </si>
-  <si>
-    <t>Few-Shot (CoT)</t>
-  </si>
-  <si>
-    <t>0..610</t>
+    <t>hints</t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4o-mini </t>
+  </si>
+  <si>
+    <t>qwen-plus</t>
+  </si>
+  <si>
+    <t>4o</t>
   </si>
 </sst>
 </file>
@@ -483,7 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -694,16 +703,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -835,8 +848,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -844,7 +860,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1203,7 +1239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ACF7E40-9809-314A-8B08-230973DFDCC8}">
   <dimension ref="B2:AT51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R21" sqref="R21:T28"/>
     </sheetView>
   </sheetViews>
@@ -1243,52 +1279,52 @@
       <c r="D3" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="82" t="s">
+      <c r="F3" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="79"/>
-      <c r="N3" s="82" t="s">
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="81"/>
+      <c r="N3" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="78"/>
-      <c r="P3" s="78"/>
-      <c r="Q3" s="78"/>
-      <c r="R3" s="78"/>
-      <c r="S3" s="78"/>
-      <c r="T3" s="79"/>
-      <c r="U3" s="78" t="s">
+      <c r="O3" s="80"/>
+      <c r="P3" s="80"/>
+      <c r="Q3" s="80"/>
+      <c r="R3" s="80"/>
+      <c r="S3" s="80"/>
+      <c r="T3" s="81"/>
+      <c r="U3" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="V3" s="78"/>
-      <c r="W3" s="78"/>
-      <c r="X3" s="78"/>
-      <c r="Y3" s="79"/>
-      <c r="Z3" s="89" t="s">
+      <c r="V3" s="80"/>
+      <c r="W3" s="80"/>
+      <c r="X3" s="80"/>
+      <c r="Y3" s="81"/>
+      <c r="Z3" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="AA3" s="87"/>
-      <c r="AB3" s="87"/>
-      <c r="AC3" s="87"/>
-      <c r="AD3" s="88"/>
-      <c r="AE3" s="86" t="s">
+      <c r="AA3" s="89"/>
+      <c r="AB3" s="89"/>
+      <c r="AC3" s="89"/>
+      <c r="AD3" s="90"/>
+      <c r="AE3" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="AF3" s="87"/>
-      <c r="AG3" s="87"/>
-      <c r="AH3" s="87"/>
-      <c r="AI3" s="88"/>
-      <c r="AJ3" s="86" t="s">
+      <c r="AF3" s="89"/>
+      <c r="AG3" s="89"/>
+      <c r="AH3" s="89"/>
+      <c r="AI3" s="90"/>
+      <c r="AJ3" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="AK3" s="87"/>
-      <c r="AL3" s="87"/>
-      <c r="AM3" s="87"/>
-      <c r="AN3" s="88"/>
+      <c r="AK3" s="89"/>
+      <c r="AL3" s="89"/>
+      <c r="AM3" s="89"/>
+      <c r="AN3" s="90"/>
       <c r="AP3" s="18"/>
       <c r="AQ3" s="21" t="s">
         <v>18</v>
@@ -1304,7 +1340,7 @@
       </c>
     </row>
     <row r="4" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="92" t="s">
+      <c r="B4" s="94" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="21">
@@ -1313,52 +1349,52 @@
       <c r="D4" s="41">
         <v>0.86699999999999999</v>
       </c>
-      <c r="F4" s="83"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80" t="s">
+      <c r="F4" s="85"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="80"/>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
-      <c r="L4" s="81"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="80"/>
-      <c r="P4" s="80" t="s">
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="83"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="80"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="80"/>
-      <c r="T4" s="81"/>
-      <c r="U4" s="80" t="s">
+      <c r="Q4" s="82"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="82"/>
+      <c r="T4" s="83"/>
+      <c r="U4" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="V4" s="80"/>
-      <c r="W4" s="80"/>
-      <c r="X4" s="80"/>
-      <c r="Y4" s="81"/>
-      <c r="Z4" s="80" t="s">
+      <c r="V4" s="82"/>
+      <c r="W4" s="82"/>
+      <c r="X4" s="82"/>
+      <c r="Y4" s="83"/>
+      <c r="Z4" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="AA4" s="80"/>
-      <c r="AB4" s="80"/>
-      <c r="AC4" s="80"/>
-      <c r="AD4" s="81"/>
-      <c r="AE4" s="80" t="s">
+      <c r="AA4" s="82"/>
+      <c r="AB4" s="82"/>
+      <c r="AC4" s="82"/>
+      <c r="AD4" s="83"/>
+      <c r="AE4" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="80"/>
-      <c r="AH4" s="80"/>
-      <c r="AI4" s="81"/>
-      <c r="AJ4" s="80" t="s">
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="82"/>
+      <c r="AH4" s="82"/>
+      <c r="AI4" s="83"/>
+      <c r="AJ4" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="AK4" s="80"/>
-      <c r="AL4" s="80"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="81"/>
+      <c r="AK4" s="82"/>
+      <c r="AL4" s="82"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="83"/>
       <c r="AP4" s="29" t="s">
         <v>48</v>
       </c>
@@ -1380,15 +1416,15 @@
       </c>
     </row>
     <row r="5" spans="2:46" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="76"/>
+      <c r="B5" s="78"/>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="25">
         <v>0.90800000000000003</v>
       </c>
-      <c r="F5" s="84"/>
-      <c r="G5" s="85"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="87"/>
       <c r="H5" s="1">
         <v>1</v>
       </c>
@@ -1405,8 +1441,8 @@
         <v>5</v>
       </c>
       <c r="M5" s="24"/>
-      <c r="N5" s="84"/>
-      <c r="O5" s="85"/>
+      <c r="N5" s="86"/>
+      <c r="O5" s="87"/>
       <c r="P5" s="1">
         <v>1</v>
       </c>
@@ -1503,14 +1539,14 @@
       </c>
     </row>
     <row r="6" spans="2:46" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="76"/>
+      <c r="B6" s="78"/>
       <c r="C6" s="1">
         <v>5</v>
       </c>
       <c r="D6" s="25">
         <v>0.94599999999999995</v>
       </c>
-      <c r="F6" s="76" t="s">
+      <c r="F6" s="78" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="1">
@@ -1532,7 +1568,7 @@
         <v>0.83740632127728898</v>
       </c>
       <c r="M6" s="24"/>
-      <c r="N6" s="76" t="s">
+      <c r="N6" s="78" t="s">
         <v>4</v>
       </c>
       <c r="O6" s="1">
@@ -1634,14 +1670,14 @@
       </c>
     </row>
     <row r="7" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="76"/>
+      <c r="B7" s="78"/>
       <c r="C7" s="1">
         <v>10</v>
       </c>
       <c r="D7" s="25">
         <v>0.94799999999999995</v>
       </c>
-      <c r="F7" s="76"/>
+      <c r="F7" s="78"/>
       <c r="G7" s="1">
         <v>2</v>
       </c>
@@ -1661,7 +1697,7 @@
         <v>0.88302400000000003</v>
       </c>
       <c r="M7" s="24"/>
-      <c r="N7" s="76"/>
+      <c r="N7" s="78"/>
       <c r="O7" s="1">
         <v>2</v>
       </c>
@@ -1742,14 +1778,14 @@
       </c>
     </row>
     <row r="8" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="77"/>
+      <c r="B8" s="79"/>
       <c r="C8" s="15">
         <v>20</v>
       </c>
       <c r="D8" s="27">
         <v>0.93400000000000005</v>
       </c>
-      <c r="F8" s="76"/>
+      <c r="F8" s="78"/>
       <c r="G8" s="1">
         <v>5</v>
       </c>
@@ -1769,7 +1805,7 @@
         <v>0.91756300000000002</v>
       </c>
       <c r="M8" s="24"/>
-      <c r="N8" s="76"/>
+      <c r="N8" s="78"/>
       <c r="O8" s="1">
         <v>5</v>
       </c>
@@ -1854,7 +1890,7 @@
       </c>
     </row>
     <row r="9" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B9" s="92" t="s">
+      <c r="B9" s="94" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="21">
@@ -1863,7 +1899,7 @@
       <c r="D9" s="41">
         <v>0.83799999999999997</v>
       </c>
-      <c r="F9" s="76"/>
+      <c r="F9" s="78"/>
       <c r="G9" s="1">
         <v>10</v>
       </c>
@@ -1883,7 +1919,7 @@
         <v>0.92538299999999996</v>
       </c>
       <c r="M9" s="24"/>
-      <c r="N9" s="76"/>
+      <c r="N9" s="78"/>
       <c r="O9" s="1">
         <v>10</v>
       </c>
@@ -1968,14 +2004,14 @@
       </c>
     </row>
     <row r="10" spans="2:46" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="76"/>
+      <c r="B10" s="78"/>
       <c r="C10" s="1">
         <v>2</v>
       </c>
       <c r="D10" s="25">
         <v>0.84699999999999998</v>
       </c>
-      <c r="F10" s="77"/>
+      <c r="F10" s="79"/>
       <c r="G10" s="15">
         <v>20</v>
       </c>
@@ -1995,7 +2031,7 @@
         <v>0.92049499999999995</v>
       </c>
       <c r="M10" s="24"/>
-      <c r="N10" s="77"/>
+      <c r="N10" s="79"/>
       <c r="O10" s="15">
         <v>20</v>
       </c>
@@ -2080,22 +2116,22 @@
       </c>
     </row>
     <row r="11" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="76"/>
+      <c r="B11" s="78"/>
       <c r="C11" s="1">
         <v>3</v>
       </c>
       <c r="D11" s="25">
         <v>0.85099999999999998</v>
       </c>
-      <c r="F11" s="83"/>
-      <c r="G11" s="80"/>
-      <c r="H11" s="80" t="s">
+      <c r="F11" s="85"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="80"/>
-      <c r="J11" s="80"/>
-      <c r="K11" s="80"/>
-      <c r="L11" s="81"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="82"/>
+      <c r="K11" s="82"/>
+      <c r="L11" s="83"/>
       <c r="M11" s="24"/>
       <c r="N11" s="42"/>
       <c r="P11" s="24"/>
@@ -2105,15 +2141,15 @@
       <c r="T11" s="24"/>
     </row>
     <row r="12" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="76"/>
+      <c r="B12" s="78"/>
       <c r="C12" s="1">
         <v>4</v>
       </c>
       <c r="D12" s="25">
         <v>0.85199999999999998</v>
       </c>
-      <c r="F12" s="84"/>
-      <c r="G12" s="85"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="87"/>
       <c r="H12" s="1">
         <v>0.1</v>
       </c>
@@ -2138,14 +2174,14 @@
       </c>
     </row>
     <row r="13" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="77"/>
+      <c r="B13" s="79"/>
       <c r="C13" s="15">
         <v>5</v>
       </c>
       <c r="D13" s="27">
         <v>0.83499999999999996</v>
       </c>
-      <c r="F13" s="76" t="s">
+      <c r="F13" s="78" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="1">
@@ -2168,7 +2204,7 @@
       </c>
     </row>
     <row r="14" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="92" t="s">
+      <c r="B14" s="94" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="21">
@@ -2177,7 +2213,7 @@
       <c r="D14" s="41">
         <v>0.65500000000000003</v>
       </c>
-      <c r="F14" s="76"/>
+      <c r="F14" s="78"/>
       <c r="G14" s="1">
         <v>2</v>
       </c>
@@ -2201,14 +2237,14 @@
       <c r="O14" s="24"/>
     </row>
     <row r="15" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B15" s="76"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="1">
         <v>0.2</v>
       </c>
       <c r="D15" s="25">
         <v>0.70099999999999996</v>
       </c>
-      <c r="F15" s="76"/>
+      <c r="F15" s="78"/>
       <c r="G15" s="1">
         <v>5</v>
       </c>
@@ -2231,14 +2267,14 @@
       <c r="P15" s="5"/>
     </row>
     <row r="16" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B16" s="76"/>
+      <c r="B16" s="78"/>
       <c r="C16" s="1">
         <v>0.3</v>
       </c>
       <c r="D16" s="25">
         <v>0.73499999999999999</v>
       </c>
-      <c r="F16" s="76"/>
+      <c r="F16" s="78"/>
       <c r="G16" s="1">
         <v>10</v>
       </c>
@@ -2260,14 +2296,14 @@
       <c r="M16" s="24"/>
     </row>
     <row r="17" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="76"/>
+      <c r="B17" s="78"/>
       <c r="C17" s="1">
         <v>0.4</v>
       </c>
       <c r="D17" s="25">
         <v>0.753</v>
       </c>
-      <c r="F17" s="77"/>
+      <c r="F17" s="79"/>
       <c r="G17" s="15">
         <v>20</v>
       </c>
@@ -2294,22 +2330,22 @@
       <c r="T17" s="24"/>
     </row>
     <row r="18" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="77"/>
+      <c r="B18" s="79"/>
       <c r="C18" s="15">
         <v>0.5</v>
       </c>
       <c r="D18" s="27">
         <v>0.65400000000000003</v>
       </c>
-      <c r="F18" s="93"/>
-      <c r="G18" s="94"/>
-      <c r="H18" s="94" t="s">
+      <c r="F18" s="95"/>
+      <c r="G18" s="96"/>
+      <c r="H18" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="94"/>
-      <c r="J18" s="94"/>
-      <c r="K18" s="94"/>
-      <c r="L18" s="97"/>
+      <c r="I18" s="96"/>
+      <c r="J18" s="96"/>
+      <c r="K18" s="96"/>
+      <c r="L18" s="99"/>
       <c r="N18" s="42"/>
       <c r="P18" s="24"/>
       <c r="Q18" s="24"/>
@@ -2318,8 +2354,8 @@
       <c r="T18" s="24"/>
     </row>
     <row r="19" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F19" s="95"/>
-      <c r="G19" s="96"/>
+      <c r="F19" s="97"/>
+      <c r="G19" s="98"/>
       <c r="H19" s="1">
         <v>0.1</v>
       </c>
@@ -2343,7 +2379,7 @@
       <c r="T19" s="24"/>
     </row>
     <row r="20" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="90" t="s">
+      <c r="F20" s="92" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="44">
@@ -2367,7 +2403,7 @@
       <c r="P20" s="24"/>
     </row>
     <row r="21" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="90"/>
+      <c r="F21" s="92"/>
       <c r="G21" s="44">
         <v>2</v>
       </c>
@@ -2388,7 +2424,7 @@
       </c>
     </row>
     <row r="22" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F22" s="90"/>
+      <c r="F22" s="92"/>
       <c r="G22" s="44">
         <v>3</v>
       </c>
@@ -2410,7 +2446,7 @@
     </row>
     <row r="23" spans="2:40" x14ac:dyDescent="0.2">
       <c r="D23" s="42"/>
-      <c r="F23" s="90"/>
+      <c r="F23" s="92"/>
       <c r="G23" s="44">
         <v>4</v>
       </c>
@@ -2434,7 +2470,7 @@
     </row>
     <row r="24" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D24" s="42"/>
-      <c r="F24" s="91"/>
+      <c r="F24" s="93"/>
       <c r="G24" s="43">
         <v>5</v>
       </c>
@@ -3023,7 +3059,7 @@
   <dimension ref="B1:W29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3044,26 +3080,26 @@
     <row r="1" spans="2:20" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B2" s="53"/>
-      <c r="D2" s="98" t="s">
+      <c r="D2" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="99" t="s">
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="100"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="102"/>
     </row>
     <row r="3" spans="2:20" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="53"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="105"/>
       <c r="H3" s="59" t="s">
         <v>54</v>
       </c>
@@ -3084,193 +3120,193 @@
       <c r="B4" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="104" t="s">
+      <c r="D4" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="105"/>
-      <c r="F4" s="109" t="s">
+      <c r="E4" s="107"/>
+      <c r="F4" s="111" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="111">
+      <c r="H4" s="113">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="111"/>
-      <c r="J4" s="111"/>
-      <c r="K4" s="111"/>
-      <c r="L4" s="112"/>
+      <c r="I4" s="113"/>
+      <c r="J4" s="113"/>
+      <c r="K4" s="113"/>
+      <c r="L4" s="114"/>
     </row>
     <row r="5" spans="2:20" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="106"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="110"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="112"/>
       <c r="G5" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="113">
+      <c r="H5" s="115">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="113"/>
-      <c r="J5" s="113"/>
-      <c r="K5" s="113"/>
-      <c r="L5" s="114"/>
+      <c r="I5" s="115"/>
+      <c r="J5" s="115"/>
+      <c r="K5" s="115"/>
+      <c r="L5" s="116"/>
     </row>
     <row r="6" spans="2:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="106"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="109" t="s">
+      <c r="D6" s="108"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="111" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="115">
+      <c r="H6" s="117">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="115"/>
-      <c r="J6" s="115"/>
-      <c r="K6" s="115"/>
-      <c r="L6" s="116"/>
+      <c r="I6" s="117"/>
+      <c r="J6" s="117"/>
+      <c r="K6" s="117"/>
+      <c r="L6" s="118"/>
     </row>
     <row r="7" spans="2:20" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="52"/>
-      <c r="D7" s="106"/>
-      <c r="E7" s="105"/>
-      <c r="F7" s="110"/>
+      <c r="D7" s="108"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="112"/>
       <c r="G7" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="113">
+      <c r="H7" s="115">
         <v>0.85199999999999998</v>
       </c>
-      <c r="I7" s="113"/>
-      <c r="J7" s="113"/>
-      <c r="K7" s="113"/>
-      <c r="L7" s="114"/>
+      <c r="I7" s="115"/>
+      <c r="J7" s="115"/>
+      <c r="K7" s="115"/>
+      <c r="L7" s="116"/>
     </row>
     <row r="8" spans="2:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="53"/>
-      <c r="D8" s="106"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="109" t="s">
+      <c r="D8" s="108"/>
+      <c r="E8" s="107"/>
+      <c r="F8" s="111" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="115">
+      <c r="H8" s="117">
         <v>0.65400000000000003</v>
       </c>
-      <c r="I8" s="115"/>
-      <c r="J8" s="115"/>
-      <c r="K8" s="115"/>
-      <c r="L8" s="116"/>
+      <c r="I8" s="117"/>
+      <c r="J8" s="117"/>
+      <c r="K8" s="117"/>
+      <c r="L8" s="118"/>
     </row>
     <row r="9" spans="2:20" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="53"/>
-      <c r="D9" s="106"/>
-      <c r="E9" s="105"/>
-      <c r="F9" s="110"/>
+      <c r="D9" s="108"/>
+      <c r="E9" s="107"/>
+      <c r="F9" s="112"/>
       <c r="G9" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="113">
+      <c r="H9" s="115">
         <v>0.753</v>
       </c>
-      <c r="I9" s="113"/>
-      <c r="J9" s="113"/>
-      <c r="K9" s="113"/>
-      <c r="L9" s="114"/>
+      <c r="I9" s="115"/>
+      <c r="J9" s="115"/>
+      <c r="K9" s="115"/>
+      <c r="L9" s="116"/>
     </row>
     <row r="10" spans="2:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="106"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="109" t="s">
+      <c r="D10" s="108"/>
+      <c r="E10" s="107"/>
+      <c r="F10" s="111" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="115">
+      <c r="H10" s="117">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I10" s="115"/>
-      <c r="J10" s="115"/>
-      <c r="K10" s="115"/>
-      <c r="L10" s="116"/>
+      <c r="I10" s="117"/>
+      <c r="J10" s="117"/>
+      <c r="K10" s="117"/>
+      <c r="L10" s="118"/>
     </row>
     <row r="11" spans="2:20" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="106"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="110"/>
+      <c r="D11" s="108"/>
+      <c r="E11" s="107"/>
+      <c r="F11" s="112"/>
       <c r="G11" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="113">
+      <c r="H11" s="115">
         <v>0.98699999999999999</v>
       </c>
-      <c r="I11" s="113"/>
-      <c r="J11" s="113"/>
-      <c r="K11" s="113"/>
-      <c r="L11" s="114"/>
+      <c r="I11" s="115"/>
+      <c r="J11" s="115"/>
+      <c r="K11" s="115"/>
+      <c r="L11" s="116"/>
     </row>
     <row r="12" spans="2:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="106"/>
-      <c r="E12" s="105"/>
-      <c r="F12" s="109" t="s">
+      <c r="D12" s="108"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="111" t="s">
         <v>21</v>
       </c>
       <c r="G12" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="115">
+      <c r="H12" s="117">
         <v>0.71499999999999997</v>
       </c>
-      <c r="I12" s="115"/>
-      <c r="J12" s="115"/>
-      <c r="K12" s="115"/>
-      <c r="L12" s="116"/>
+      <c r="I12" s="117"/>
+      <c r="J12" s="117"/>
+      <c r="K12" s="117"/>
+      <c r="L12" s="118"/>
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
     <row r="13" spans="2:20" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="107"/>
-      <c r="E13" s="108"/>
-      <c r="F13" s="117"/>
+      <c r="D13" s="109"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="119"/>
       <c r="G13" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="111">
+      <c r="H13" s="113">
         <v>0.99</v>
       </c>
-      <c r="I13" s="111"/>
-      <c r="J13" s="111"/>
-      <c r="K13" s="111"/>
-      <c r="L13" s="112"/>
+      <c r="I13" s="113"/>
+      <c r="J13" s="113"/>
+      <c r="K13" s="113"/>
+      <c r="L13" s="114"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
     </row>
     <row r="14" spans="2:20" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="118" t="s">
+      <c r="D14" s="120" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="109" t="s">
+      <c r="E14" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="82" t="s">
+      <c r="F14" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="79"/>
+      <c r="G14" s="81"/>
       <c r="H14" s="67">
         <v>0.52</v>
       </c>
@@ -3287,31 +3323,31 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="O14" s="31"/>
-      <c r="P14" s="122">
+      <c r="P14" s="72">
         <f>AVERAGE(H15:H21)</f>
         <v>0.52228571428571435</v>
       </c>
-      <c r="Q14" s="122">
+      <c r="Q14" s="72">
         <f t="shared" ref="Q14:T14" si="0">AVERAGE(I15:I21)</f>
         <v>0.59928571428571431</v>
       </c>
-      <c r="R14" s="122">
+      <c r="R14" s="72">
         <f t="shared" si="0"/>
         <v>0.49414285714285722</v>
       </c>
-      <c r="S14" s="122">
+      <c r="S14" s="72">
         <f t="shared" si="0"/>
         <v>0.64857142857142858</v>
       </c>
-      <c r="T14" s="122">
+      <c r="T14" s="72">
         <f t="shared" si="0"/>
         <v>0.44528571428571434</v>
       </c>
     </row>
     <row r="15" spans="2:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="106"/>
-      <c r="E15" s="117"/>
-      <c r="F15" s="117" t="s">
+      <c r="D15" s="108"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="119" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -3333,31 +3369,31 @@
         <v>0.54600000000000004</v>
       </c>
       <c r="O15" s="31"/>
-      <c r="P15" s="122">
+      <c r="P15" s="72">
         <f>AVERAGE(H23:H29)</f>
         <v>0.49157142857142855</v>
       </c>
-      <c r="Q15" s="122">
+      <c r="Q15" s="72">
         <f t="shared" ref="Q15:T15" si="1">AVERAGE(I23:I29)</f>
         <v>0.6012857142857142</v>
       </c>
-      <c r="R15" s="122">
+      <c r="R15" s="72">
         <f t="shared" si="1"/>
         <v>0.56214285714285717</v>
       </c>
-      <c r="S15" s="122">
+      <c r="S15" s="72">
         <f t="shared" si="1"/>
         <v>0.66142857142857159</v>
       </c>
-      <c r="T15" s="122">
+      <c r="T15" s="72">
         <f t="shared" si="1"/>
         <v>0.58542857142857141</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D16" s="106"/>
-      <c r="E16" s="117"/>
-      <c r="F16" s="117"/>
+      <c r="D16" s="108"/>
+      <c r="E16" s="119"/>
+      <c r="F16" s="119"/>
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
@@ -3383,9 +3419,9 @@
       <c r="S16" s="31"/>
     </row>
     <row r="17" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D17" s="106"/>
-      <c r="E17" s="117"/>
-      <c r="F17" s="117"/>
+      <c r="D17" s="108"/>
+      <c r="E17" s="119"/>
+      <c r="F17" s="119"/>
       <c r="G17" s="1" t="s">
         <v>22</v>
       </c>
@@ -3412,9 +3448,9 @@
       <c r="W17" s="5"/>
     </row>
     <row r="18" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D18" s="106"/>
-      <c r="E18" s="117"/>
-      <c r="F18" s="117"/>
+      <c r="D18" s="108"/>
+      <c r="E18" s="119"/>
+      <c r="F18" s="119"/>
       <c r="G18" s="1" t="s">
         <v>45</v>
       </c>
@@ -3440,9 +3476,9 @@
       <c r="S18" s="31"/>
     </row>
     <row r="19" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D19" s="106"/>
-      <c r="E19" s="117"/>
-      <c r="F19" s="117"/>
+      <c r="D19" s="108"/>
+      <c r="E19" s="119"/>
+      <c r="F19" s="119"/>
       <c r="G19" s="1" t="s">
         <v>46</v>
       </c>
@@ -3468,9 +3504,9 @@
       <c r="S19" s="31"/>
     </row>
     <row r="20" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D20" s="106"/>
-      <c r="E20" s="117"/>
-      <c r="F20" s="117"/>
+      <c r="D20" s="108"/>
+      <c r="E20" s="119"/>
+      <c r="F20" s="119"/>
       <c r="G20" s="1" t="s">
         <v>47</v>
       </c>
@@ -3496,9 +3532,9 @@
       <c r="S20" s="31"/>
     </row>
     <row r="21" spans="4:23" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="106"/>
-      <c r="E21" s="117"/>
-      <c r="F21" s="110"/>
+      <c r="D21" s="108"/>
+      <c r="E21" s="119"/>
+      <c r="F21" s="112"/>
       <c r="G21" s="15" t="s">
         <v>21</v>
       </c>
@@ -3524,14 +3560,14 @@
       <c r="S21" s="31"/>
     </row>
     <row r="22" spans="4:23" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="106"/>
-      <c r="E22" s="109" t="s">
+      <c r="D22" s="108"/>
+      <c r="E22" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="F22" s="82" t="s">
+      <c r="F22" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="79"/>
+      <c r="G22" s="81"/>
       <c r="H22" s="68">
         <v>0.495</v>
       </c>
@@ -3554,9 +3590,9 @@
       <c r="S22" s="31"/>
     </row>
     <row r="23" spans="4:23" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="106"/>
-      <c r="E23" s="117"/>
-      <c r="F23" s="117" t="s">
+      <c r="D23" s="108"/>
+      <c r="E23" s="119"/>
+      <c r="F23" s="119" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -3584,9 +3620,9 @@
       <c r="S23" s="31"/>
     </row>
     <row r="24" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D24" s="106"/>
-      <c r="E24" s="117"/>
-      <c r="F24" s="117"/>
+      <c r="D24" s="108"/>
+      <c r="E24" s="119"/>
+      <c r="F24" s="119"/>
       <c r="G24" s="1" t="s">
         <v>12</v>
       </c>
@@ -3612,9 +3648,9 @@
       <c r="S24" s="31"/>
     </row>
     <row r="25" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D25" s="106"/>
-      <c r="E25" s="117"/>
-      <c r="F25" s="117"/>
+      <c r="D25" s="108"/>
+      <c r="E25" s="119"/>
+      <c r="F25" s="119"/>
       <c r="G25" s="1" t="s">
         <v>22</v>
       </c>
@@ -3640,9 +3676,9 @@
       <c r="S25" s="31"/>
     </row>
     <row r="26" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D26" s="106"/>
-      <c r="E26" s="117"/>
-      <c r="F26" s="117"/>
+      <c r="D26" s="108"/>
+      <c r="E26" s="119"/>
+      <c r="F26" s="119"/>
       <c r="G26" s="1" t="s">
         <v>45</v>
       </c>
@@ -3668,9 +3704,9 @@
       <c r="S26" s="31"/>
     </row>
     <row r="27" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D27" s="106"/>
-      <c r="E27" s="117"/>
-      <c r="F27" s="117"/>
+      <c r="D27" s="108"/>
+      <c r="E27" s="119"/>
+      <c r="F27" s="119"/>
       <c r="G27" s="1" t="s">
         <v>46</v>
       </c>
@@ -3696,9 +3732,9 @@
       <c r="S27" s="31"/>
     </row>
     <row r="28" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D28" s="106"/>
-      <c r="E28" s="117"/>
-      <c r="F28" s="117"/>
+      <c r="D28" s="108"/>
+      <c r="E28" s="119"/>
+      <c r="F28" s="119"/>
       <c r="G28" s="1" t="s">
         <v>47</v>
       </c>
@@ -3724,9 +3760,9 @@
       <c r="S28" s="31"/>
     </row>
     <row r="29" spans="4:23" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="107"/>
-      <c r="E29" s="110"/>
-      <c r="F29" s="110"/>
+      <c r="D29" s="109"/>
+      <c r="E29" s="112"/>
+      <c r="F29" s="112"/>
       <c r="G29" s="15" t="s">
         <v>21</v>
       </c>
@@ -3798,10 +3834,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B202F2B-277F-994F-8FBA-31A55EB8F243}">
-  <dimension ref="B1:U41"/>
+  <dimension ref="B1:U27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3822,26 +3858,26 @@
     <row r="1" spans="2:21" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B2" s="53"/>
-      <c r="D2" s="98" t="s">
+      <c r="D2" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="99" t="s">
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="100"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="102"/>
     </row>
     <row r="3" spans="2:21" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="53"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="105"/>
       <c r="H3" s="59" t="s">
         <v>54</v>
       </c>
@@ -3862,184 +3898,184 @@
       <c r="B4" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="104" t="s">
+      <c r="D4" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="105"/>
-      <c r="F4" s="109" t="s">
+      <c r="E4" s="107"/>
+      <c r="F4" s="111" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="111">
+      <c r="H4" s="113">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="111"/>
-      <c r="J4" s="111"/>
-      <c r="K4" s="111"/>
-      <c r="L4" s="112"/>
+      <c r="I4" s="113"/>
+      <c r="J4" s="113"/>
+      <c r="K4" s="113"/>
+      <c r="L4" s="114"/>
     </row>
     <row r="5" spans="2:21" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="106"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="110"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="112"/>
       <c r="G5" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="113">
+      <c r="H5" s="115">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="113"/>
-      <c r="J5" s="113"/>
-      <c r="K5" s="113"/>
-      <c r="L5" s="114"/>
+      <c r="I5" s="115"/>
+      <c r="J5" s="115"/>
+      <c r="K5" s="115"/>
+      <c r="L5" s="116"/>
     </row>
     <row r="6" spans="2:21" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="106"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="109" t="s">
+      <c r="D6" s="108"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="111" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="115">
+      <c r="H6" s="117">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="115"/>
-      <c r="J6" s="115"/>
-      <c r="K6" s="115"/>
-      <c r="L6" s="116"/>
+      <c r="I6" s="117"/>
+      <c r="J6" s="117"/>
+      <c r="K6" s="117"/>
+      <c r="L6" s="118"/>
     </row>
     <row r="7" spans="2:21" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="52"/>
-      <c r="D7" s="106"/>
-      <c r="E7" s="105"/>
-      <c r="F7" s="110"/>
+      <c r="D7" s="108"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="112"/>
       <c r="G7" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="113">
+      <c r="H7" s="115">
         <v>0.85199999999999998</v>
       </c>
-      <c r="I7" s="113"/>
-      <c r="J7" s="113"/>
-      <c r="K7" s="113"/>
-      <c r="L7" s="114"/>
+      <c r="I7" s="115"/>
+      <c r="J7" s="115"/>
+      <c r="K7" s="115"/>
+      <c r="L7" s="116"/>
     </row>
     <row r="8" spans="2:21" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="53"/>
-      <c r="D8" s="106"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="109" t="s">
+      <c r="D8" s="108"/>
+      <c r="E8" s="107"/>
+      <c r="F8" s="111" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="115">
+      <c r="H8" s="117">
         <v>0.65400000000000003</v>
       </c>
-      <c r="I8" s="115"/>
-      <c r="J8" s="115"/>
-      <c r="K8" s="115"/>
-      <c r="L8" s="116"/>
+      <c r="I8" s="117"/>
+      <c r="J8" s="117"/>
+      <c r="K8" s="117"/>
+      <c r="L8" s="118"/>
     </row>
     <row r="9" spans="2:21" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="53"/>
-      <c r="D9" s="106"/>
-      <c r="E9" s="105"/>
-      <c r="F9" s="110"/>
+      <c r="D9" s="108"/>
+      <c r="E9" s="107"/>
+      <c r="F9" s="112"/>
       <c r="G9" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="113">
+      <c r="H9" s="115">
         <v>0.753</v>
       </c>
-      <c r="I9" s="113"/>
-      <c r="J9" s="113"/>
-      <c r="K9" s="113"/>
-      <c r="L9" s="114"/>
+      <c r="I9" s="115"/>
+      <c r="J9" s="115"/>
+      <c r="K9" s="115"/>
+      <c r="L9" s="116"/>
     </row>
     <row r="10" spans="2:21" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="106"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="109" t="s">
+      <c r="D10" s="108"/>
+      <c r="E10" s="107"/>
+      <c r="F10" s="111" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="115">
+      <c r="H10" s="117">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I10" s="115"/>
-      <c r="J10" s="115"/>
-      <c r="K10" s="115"/>
-      <c r="L10" s="116"/>
+      <c r="I10" s="117"/>
+      <c r="J10" s="117"/>
+      <c r="K10" s="117"/>
+      <c r="L10" s="118"/>
     </row>
     <row r="11" spans="2:21" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="106"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="110"/>
+      <c r="D11" s="108"/>
+      <c r="E11" s="107"/>
+      <c r="F11" s="112"/>
       <c r="G11" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="113">
+      <c r="H11" s="115">
         <v>0.98699999999999999</v>
       </c>
-      <c r="I11" s="113"/>
-      <c r="J11" s="113"/>
-      <c r="K11" s="113"/>
-      <c r="L11" s="114"/>
+      <c r="I11" s="115"/>
+      <c r="J11" s="115"/>
+      <c r="K11" s="115"/>
+      <c r="L11" s="116"/>
     </row>
     <row r="12" spans="2:21" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="106"/>
-      <c r="E12" s="105"/>
-      <c r="F12" s="109" t="s">
+      <c r="D12" s="108"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="111" t="s">
         <v>21</v>
       </c>
       <c r="G12" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="115">
+      <c r="H12" s="117">
         <v>0.71499999999999997</v>
       </c>
-      <c r="I12" s="115"/>
-      <c r="J12" s="115"/>
-      <c r="K12" s="115"/>
-      <c r="L12" s="116"/>
+      <c r="I12" s="117"/>
+      <c r="J12" s="117"/>
+      <c r="K12" s="117"/>
+      <c r="L12" s="118"/>
     </row>
     <row r="13" spans="2:21" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="107"/>
-      <c r="E13" s="108"/>
-      <c r="F13" s="117"/>
+      <c r="D13" s="109"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="119"/>
       <c r="G13" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="111">
+      <c r="H13" s="113">
         <v>0.99</v>
       </c>
-      <c r="I13" s="111"/>
-      <c r="J13" s="111"/>
-      <c r="K13" s="111"/>
-      <c r="L13" s="112"/>
+      <c r="I13" s="113"/>
+      <c r="J13" s="113"/>
+      <c r="K13" s="113"/>
+      <c r="L13" s="114"/>
     </row>
     <row r="14" spans="2:21" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="106" t="s">
+      <c r="D14" s="111" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="106" t="s">
+      <c r="E14" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="109" t="s">
+      <c r="F14" s="111" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="21" t="s">
@@ -4083,9 +4119,9 @@
       <c r="U14" s="5"/>
     </row>
     <row r="15" spans="2:21" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="106"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="117"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="108"/>
+      <c r="F15" s="119"/>
       <c r="G15" s="1" t="s">
         <v>12</v>
       </c>
@@ -4105,11 +4141,11 @@
         <v>0.67</v>
       </c>
       <c r="P15" s="5">
-        <f>AVERAGE(H28:H34)</f>
+        <f>AVERAGE(H21:H27)</f>
         <v>0.51728571428571424</v>
       </c>
       <c r="Q15" s="5">
-        <f t="shared" ref="Q15:T15" si="1">AVERAGE(I28:I34)</f>
+        <f t="shared" ref="Q15:T15" si="1">AVERAGE(I21:I27)</f>
         <v>0.64242857142857146</v>
       </c>
       <c r="R15" s="5">
@@ -4127,9 +4163,9 @@
       <c r="U15" s="5"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="D16" s="106"/>
-      <c r="E16" s="106"/>
-      <c r="F16" s="117"/>
+      <c r="D16" s="119"/>
+      <c r="E16" s="108"/>
+      <c r="F16" s="119"/>
       <c r="G16" s="1" t="s">
         <v>22</v>
       </c>
@@ -4150,9 +4186,9 @@
       </c>
     </row>
     <row r="17" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D17" s="106"/>
-      <c r="E17" s="106"/>
-      <c r="F17" s="117"/>
+      <c r="D17" s="119"/>
+      <c r="E17" s="108"/>
+      <c r="F17" s="119"/>
       <c r="G17" s="1" t="s">
         <v>45</v>
       </c>
@@ -4178,9 +4214,9 @@
       <c r="U17" s="5"/>
     </row>
     <row r="18" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D18" s="106"/>
-      <c r="E18" s="106"/>
-      <c r="F18" s="117"/>
+      <c r="D18" s="119"/>
+      <c r="E18" s="108"/>
+      <c r="F18" s="119"/>
       <c r="G18" s="1" t="s">
         <v>46</v>
       </c>
@@ -4201,9 +4237,9 @@
       </c>
     </row>
     <row r="19" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D19" s="106"/>
-      <c r="E19" s="106"/>
-      <c r="F19" s="117"/>
+      <c r="D19" s="119"/>
+      <c r="E19" s="108"/>
+      <c r="F19" s="119"/>
       <c r="G19" s="1" t="s">
         <v>47</v>
       </c>
@@ -4227,9 +4263,9 @@
       <c r="Q19" s="5"/>
     </row>
     <row r="20" spans="4:21" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="106"/>
-      <c r="E20" s="107"/>
-      <c r="F20" s="110"/>
+      <c r="D20" s="119"/>
+      <c r="E20" s="109"/>
+      <c r="F20" s="112"/>
       <c r="G20" s="15" t="s">
         <v>21</v>
       </c>
@@ -4250,479 +4286,172 @@
       </c>
     </row>
     <row r="21" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D21" s="106"/>
-      <c r="E21" s="109" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" s="109" t="s">
+      <c r="D21" s="119"/>
+      <c r="E21" s="111" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="G21" s="21" t="s">
+      <c r="G21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H21" s="67"/>
-      <c r="I21" s="54">
-        <v>0.68200000000000005</v>
-      </c>
-      <c r="J21" s="54">
-        <v>0.94199999999999995</v>
-      </c>
-      <c r="K21" s="54">
-        <v>0.92100000000000004</v>
-      </c>
-      <c r="L21" s="55">
-        <v>0.94699999999999995</v>
+      <c r="H21" s="68">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="I21" s="6">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="J21" s="6">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="K21" s="6">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="L21" s="14">
+        <v>0.93100000000000005</v>
       </c>
     </row>
     <row r="22" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D22" s="106"/>
-      <c r="E22" s="117"/>
-      <c r="F22" s="117"/>
+      <c r="D22" s="119"/>
+      <c r="E22" s="119"/>
+      <c r="F22" s="119"/>
       <c r="G22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="68"/>
+      <c r="H22" s="68">
+        <v>0.48499999999999999</v>
+      </c>
       <c r="I22" s="6">
-        <v>0.59899999999999998</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="J22" s="6">
-        <v>0.61599999999999999</v>
+        <v>0.82199999999999995</v>
       </c>
       <c r="K22" s="6">
-        <v>0.72299999999999998</v>
+        <v>0.84499999999999997</v>
       </c>
       <c r="L22" s="14">
-        <v>0.74199999999999999</v>
+        <v>0.83699999999999997</v>
       </c>
     </row>
     <row r="23" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D23" s="106"/>
-      <c r="E23" s="117"/>
-      <c r="F23" s="117"/>
+      <c r="D23" s="119"/>
+      <c r="E23" s="119"/>
+      <c r="F23" s="119"/>
       <c r="G23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="68"/>
+      <c r="H23" s="68">
+        <v>0.505</v>
+      </c>
       <c r="I23" s="6">
-        <v>0.59899999999999998</v>
+        <v>0.65700000000000003</v>
       </c>
       <c r="J23" s="6">
-        <v>0.60199999999999998</v>
+        <v>0.76</v>
       </c>
       <c r="K23" s="6">
-        <v>0.60499999999999998</v>
+        <v>0.68700000000000006</v>
       </c>
       <c r="L23" s="14">
-        <v>0.64300000000000002</v>
+        <v>0.72699999999999998</v>
       </c>
     </row>
     <row r="24" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D24" s="106"/>
-      <c r="E24" s="117"/>
-      <c r="F24" s="117"/>
+      <c r="D24" s="119"/>
+      <c r="E24" s="119"/>
+      <c r="F24" s="119"/>
       <c r="G24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H24" s="68"/>
+      <c r="H24" s="68">
+        <v>0.51700000000000002</v>
+      </c>
       <c r="I24" s="6">
-        <v>0.63400000000000001</v>
+        <v>0.67600000000000005</v>
       </c>
       <c r="J24" s="6">
-        <v>0.94599999999999995</v>
+        <v>0.91600000000000004</v>
       </c>
       <c r="K24" s="6">
-        <v>0.92700000000000005</v>
+        <v>0.94099999999999995</v>
       </c>
       <c r="L24" s="14">
-        <v>0.95</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="25" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D25" s="106"/>
-      <c r="E25" s="117"/>
-      <c r="F25" s="117"/>
+      <c r="D25" s="119"/>
+      <c r="E25" s="119"/>
+      <c r="F25" s="119"/>
       <c r="G25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H25" s="68"/>
+      <c r="H25" s="68">
+        <v>0.47899999999999998</v>
+      </c>
       <c r="I25" s="6">
-        <v>0.59899999999999998</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="J25" s="6">
-        <v>0.92</v>
+        <v>0.85799999999999998</v>
       </c>
       <c r="K25" s="6">
-        <v>0.88700000000000001</v>
+        <v>0.96799999999999997</v>
       </c>
       <c r="L25" s="14">
-        <v>0.96299999999999997</v>
+        <v>0.95899999999999996</v>
       </c>
     </row>
     <row r="26" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D26" s="106"/>
-      <c r="E26" s="117"/>
-      <c r="F26" s="117"/>
+      <c r="D26" s="119"/>
+      <c r="E26" s="119"/>
+      <c r="F26" s="119"/>
       <c r="G26" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H26" s="68"/>
+      <c r="H26" s="68">
+        <v>0.49</v>
+      </c>
       <c r="I26" s="6">
-        <v>0.60699999999999998</v>
+        <v>0.45700000000000002</v>
       </c>
       <c r="J26" s="6">
-        <v>0.73199999999999998</v>
+        <v>0.90600000000000003</v>
       </c>
       <c r="K26" s="6">
-        <v>0.72499999999999998</v>
+        <v>0.94799999999999995</v>
       </c>
       <c r="L26" s="14">
-        <v>0.80700000000000005</v>
-      </c>
-      <c r="Q26" s="5"/>
+        <v>0.93899999999999995</v>
+      </c>
     </row>
     <row r="27" spans="4:21" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="106"/>
-      <c r="E27" s="117"/>
-      <c r="F27" s="110"/>
+      <c r="D27" s="112"/>
+      <c r="E27" s="112"/>
+      <c r="F27" s="112"/>
       <c r="G27" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="H27" s="69"/>
+      <c r="H27" s="69">
+        <v>0.53900000000000003</v>
+      </c>
       <c r="I27" s="16">
-        <v>0.60299999999999998</v>
+        <v>0.625</v>
       </c>
       <c r="J27" s="16">
-        <v>0.91400000000000003</v>
+        <v>0.872</v>
       </c>
       <c r="K27" s="16">
-        <v>0.78900000000000003</v>
+        <v>0.98399999999999999</v>
       </c>
       <c r="L27" s="17">
-        <v>0.95399999999999996</v>
-      </c>
-      <c r="Q27" s="5"/>
-    </row>
-    <row r="28" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D28" s="106"/>
-      <c r="E28" s="109" t="s">
-        <v>2</v>
-      </c>
-      <c r="F28" s="109" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H28" s="68">
-        <v>0.60599999999999998</v>
-      </c>
-      <c r="I28" s="6">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="J28" s="6">
-        <v>0.92900000000000005</v>
-      </c>
-      <c r="K28" s="6">
-        <v>0.93600000000000005</v>
-      </c>
-      <c r="L28" s="14">
-        <v>0.93100000000000005</v>
-      </c>
-    </row>
-    <row r="29" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D29" s="106"/>
-      <c r="E29" s="117"/>
-      <c r="F29" s="117"/>
-      <c r="G29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" s="68">
-        <v>0.48499999999999999</v>
-      </c>
-      <c r="I29" s="6">
-        <v>0.59699999999999998</v>
-      </c>
-      <c r="J29" s="6">
-        <v>0.82199999999999995</v>
-      </c>
-      <c r="K29" s="6">
-        <v>0.84499999999999997</v>
-      </c>
-      <c r="L29" s="14">
-        <v>0.83699999999999997</v>
-      </c>
-    </row>
-    <row r="30" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D30" s="106"/>
-      <c r="E30" s="117"/>
-      <c r="F30" s="117"/>
-      <c r="G30" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H30" s="68">
-        <v>0.505</v>
-      </c>
-      <c r="I30" s="6">
-        <v>0.65700000000000003</v>
-      </c>
-      <c r="J30" s="6">
-        <v>0.76</v>
-      </c>
-      <c r="K30" s="6">
-        <v>0.68700000000000006</v>
-      </c>
-      <c r="L30" s="14">
-        <v>0.72699999999999998</v>
-      </c>
-    </row>
-    <row r="31" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D31" s="106"/>
-      <c r="E31" s="117"/>
-      <c r="F31" s="117"/>
-      <c r="G31" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H31" s="68">
-        <v>0.51700000000000002</v>
-      </c>
-      <c r="I31" s="6">
-        <v>0.67600000000000005</v>
-      </c>
-      <c r="J31" s="6">
-        <v>0.91600000000000004</v>
-      </c>
-      <c r="K31" s="6">
-        <v>0.94099999999999995</v>
-      </c>
-      <c r="L31" s="14">
-        <v>0.94</v>
-      </c>
-    </row>
-    <row r="32" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D32" s="106"/>
-      <c r="E32" s="117"/>
-      <c r="F32" s="117"/>
-      <c r="G32" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H32" s="68">
-        <v>0.47899999999999998</v>
-      </c>
-      <c r="I32" s="6">
-        <v>0.61799999999999999</v>
-      </c>
-      <c r="J32" s="6">
-        <v>0.85799999999999998</v>
-      </c>
-      <c r="K32" s="6">
-        <v>0.96799999999999997</v>
-      </c>
-      <c r="L32" s="14">
-        <v>0.95899999999999996</v>
-      </c>
-    </row>
-    <row r="33" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D33" s="106"/>
-      <c r="E33" s="117"/>
-      <c r="F33" s="117"/>
-      <c r="G33" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H33" s="68">
-        <v>0.49</v>
-      </c>
-      <c r="I33" s="6">
-        <v>0.45700000000000002</v>
-      </c>
-      <c r="J33" s="6">
-        <v>0.90600000000000003</v>
-      </c>
-      <c r="K33" s="6">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="L33" s="14">
-        <v>0.93899999999999995</v>
-      </c>
-    </row>
-    <row r="34" spans="4:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D34" s="106"/>
-      <c r="E34" s="110"/>
-      <c r="F34" s="110"/>
-      <c r="G34" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H34" s="69">
-        <v>0.53900000000000003</v>
-      </c>
-      <c r="I34" s="16">
-        <v>0.625</v>
-      </c>
-      <c r="J34" s="16">
-        <v>0.872</v>
-      </c>
-      <c r="K34" s="16">
-        <v>0.98399999999999999</v>
-      </c>
-      <c r="L34" s="17">
         <v>0.96699999999999997</v>
       </c>
     </row>
-    <row r="35" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D35" s="106"/>
-      <c r="E35" s="106" t="s">
-        <v>56</v>
-      </c>
-      <c r="F35" s="109" t="s">
-        <v>10</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H35" s="68"/>
-      <c r="I35" s="6">
-        <v>0.93899999999999995</v>
-      </c>
-      <c r="J35" s="6">
-        <v>0.92200000000000004</v>
-      </c>
-      <c r="K35" s="6">
-        <v>0.93500000000000005</v>
-      </c>
-      <c r="L35" s="14">
-        <v>0.93700000000000006</v>
-      </c>
-      <c r="O35" s="5"/>
-      <c r="P35" s="5"/>
-      <c r="Q35" s="5"/>
-    </row>
-    <row r="36" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D36" s="106"/>
-      <c r="E36" s="106"/>
-      <c r="F36" s="117"/>
-      <c r="G36" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H36" s="68"/>
-      <c r="I36" s="6">
-        <v>0.54</v>
-      </c>
-      <c r="J36" s="6">
-        <v>0.80700000000000005</v>
-      </c>
-      <c r="K36" s="6">
-        <v>0.81599999999999995</v>
-      </c>
-      <c r="L36" s="14">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="37" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D37" s="106"/>
-      <c r="E37" s="106"/>
-      <c r="F37" s="117"/>
-      <c r="G37" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H37" s="68"/>
-      <c r="I37" s="6">
-        <v>0.66900000000000004</v>
-      </c>
-      <c r="J37" s="6">
-        <v>0.749</v>
-      </c>
-      <c r="K37" s="6">
-        <v>0.71599999999999997</v>
-      </c>
-      <c r="L37" s="14">
-        <v>0.71699999999999997</v>
-      </c>
-    </row>
-    <row r="38" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D38" s="106"/>
-      <c r="E38" s="106"/>
-      <c r="F38" s="117"/>
-      <c r="G38" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H38" s="68"/>
-      <c r="I38" s="6">
-        <v>0.57699999999999996</v>
-      </c>
-      <c r="J38" s="6">
-        <v>0.94299999999999995</v>
-      </c>
-      <c r="K38" s="6">
-        <v>0.93500000000000005</v>
-      </c>
-      <c r="L38" s="14">
-        <v>0.94399999999999995</v>
-      </c>
-    </row>
-    <row r="39" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D39" s="106"/>
-      <c r="E39" s="106"/>
-      <c r="F39" s="117"/>
-      <c r="G39" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H39" s="68"/>
-      <c r="I39" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="J39" s="6">
-        <v>0.95499999999999996</v>
-      </c>
-      <c r="K39" s="6">
-        <v>0.96299999999999997</v>
-      </c>
-      <c r="L39" s="14">
-        <v>0.97099999999999997</v>
-      </c>
-    </row>
-    <row r="40" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D40" s="106"/>
-      <c r="E40" s="106"/>
-      <c r="F40" s="117"/>
-      <c r="G40" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H40" s="68"/>
-      <c r="I40" s="6">
-        <v>0.34100000000000003</v>
-      </c>
-      <c r="J40" s="6">
-        <v>0.89800000000000002</v>
-      </c>
-      <c r="K40" s="6">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="L40" s="14">
-        <v>0.92100000000000004</v>
-      </c>
-    </row>
-    <row r="41" spans="4:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="107"/>
-      <c r="E41" s="107"/>
-      <c r="F41" s="110"/>
-      <c r="G41" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H41" s="69"/>
-      <c r="I41" s="16">
-        <v>0.60899999999999999</v>
-      </c>
-      <c r="J41" s="16">
-        <v>0.96499999999999997</v>
-      </c>
-      <c r="K41" s="16">
-        <v>0.90300000000000002</v>
-      </c>
-      <c r="L41" s="17">
-        <v>0.97699999999999998</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="23">
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D4:E13"/>
@@ -4741,18 +4470,14 @@
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="H10:L10"/>
     <mergeCell ref="H11:L11"/>
-    <mergeCell ref="F35:F41"/>
-    <mergeCell ref="D14:D41"/>
+    <mergeCell ref="D14:D27"/>
     <mergeCell ref="E14:E20"/>
     <mergeCell ref="F14:F20"/>
-    <mergeCell ref="E35:E41"/>
     <mergeCell ref="E21:E27"/>
     <mergeCell ref="F21:F27"/>
-    <mergeCell ref="E28:E34"/>
-    <mergeCell ref="F28:F34"/>
   </mergeCells>
-  <conditionalFormatting sqref="H4:L41">
-    <cfRule type="colorScale" priority="53">
+  <conditionalFormatting sqref="H4:L27">
+    <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4770,10 +4495,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D718D1-05D9-2146-B7ED-D601D310FD08}">
-  <dimension ref="B1:H20"/>
+  <dimension ref="B1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -4783,293 +4508,313 @@
     <col min="3" max="3" width="6.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="2:8" ht="41" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="120"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="70" t="s">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="2:11" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="123"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="70" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="70" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="71" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="84" t="s">
+      <c r="F2" s="128" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="129"/>
+      <c r="H2" s="128" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="129"/>
+      <c r="J2" s="130" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" s="129"/>
+    </row>
+    <row r="3" spans="2:11" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="125"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3" s="71" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C4" s="123" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="127"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="71"/>
+    </row>
+    <row r="5" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="86" t="s">
         <v>48</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="72">
-        <v>0.65400000000000003</v>
-      </c>
-      <c r="F3" s="21">
-        <v>0.94499999999999995</v>
-      </c>
-      <c r="G3" s="21">
-        <v>0.95699999999999996</v>
-      </c>
-      <c r="H3" s="22">
-        <v>0.99199999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="84"/>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="73">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.96599999999999997</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0.97399999999999998</v>
-      </c>
-      <c r="H4" s="23">
-        <v>0.97599999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="84" t="s">
-        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="73">
-        <v>0.73499999999999999</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="E5" s="75">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="23">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="I5" s="23">
         <v>0.95699999999999996</v>
       </c>
-      <c r="G5" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="H5" s="23">
-        <v>0.995</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C6" s="84"/>
+      <c r="K5" s="23">
+        <v>0.99199999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="86"/>
       <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="73">
+      <c r="E6" s="75">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="23">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="I6" s="23">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="K6" s="23">
+        <v>0.97599999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="86" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="75">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="23">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="I7" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="K7" s="23">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C8" s="86"/>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="75">
         <v>0.98699999999999999</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F8" s="5"/>
+      <c r="G8" s="23">
         <v>0.95199999999999996</v>
       </c>
-      <c r="G6" s="1">
+      <c r="I8" s="23">
         <v>0.98799999999999999</v>
       </c>
-      <c r="H6" s="13">
+      <c r="K8" s="13">
         <v>0.99</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="84" t="s">
+    <row r="9" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D9" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="74">
+      <c r="E9" s="76">
         <v>0.71499999999999997</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F9" s="45"/>
+      <c r="G9" s="23">
         <v>0.96099999999999997</v>
       </c>
-      <c r="G7" s="1">
+      <c r="I9" s="23">
         <v>0.94399999999999995</v>
       </c>
-      <c r="H7" s="23">
+      <c r="K9" s="23">
         <v>0.98899999999999999</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="119"/>
-      <c r="D8" s="43" t="s">
+    <row r="10" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="131"/>
+      <c r="D10" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="75">
+      <c r="E10" s="77">
         <v>0.99</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F10" s="73"/>
+      <c r="G10" s="66">
         <v>0.95499999999999996</v>
       </c>
-      <c r="G8" s="15">
+      <c r="H10" s="15"/>
+      <c r="I10" s="66">
         <v>0.98899999999999999</v>
       </c>
-      <c r="H8" s="66">
+      <c r="J10" s="15"/>
+      <c r="K10" s="66">
         <v>0.99399999999999999</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="F10" s="5">
-        <f>(F3-$E3)/$E3</f>
-        <v>0.44495412844036686</v>
-      </c>
-      <c r="G10" s="5">
-        <f t="shared" ref="G10:H10" si="0">(G3-$E3)/$E3</f>
-        <v>0.46330275229357787</v>
-      </c>
-      <c r="H10" s="5">
-        <f t="shared" si="0"/>
-        <v>0.51681957186544336</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="F11" s="5">
-        <f t="shared" ref="F11:H15" si="1">(F4-$E4)/$E4</f>
-        <v>1.8987341772151917E-2</v>
-      </c>
-      <c r="G11" s="5">
-        <f t="shared" si="1"/>
-        <v>2.7426160337552768E-2</v>
-      </c>
-      <c r="H11" s="5">
-        <f t="shared" si="1"/>
-        <v>2.9535864978902981E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="F12" s="5">
-        <f t="shared" si="1"/>
-        <v>0.30204081632653057</v>
-      </c>
-      <c r="G12" s="5">
-        <f t="shared" si="1"/>
-        <v>0.29251700680272102</v>
-      </c>
-      <c r="H12" s="5">
-        <f t="shared" si="1"/>
-        <v>0.35374149659863946</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="F13" s="5">
-        <f t="shared" si="1"/>
-        <v>-3.5460992907801449E-2</v>
-      </c>
-      <c r="G13" s="5">
-        <f t="shared" si="1"/>
-        <v>1.0131712259371843E-3</v>
-      </c>
-      <c r="H13" s="5">
-        <f t="shared" si="1"/>
-        <v>3.0395136778115527E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="F14" s="5">
-        <f t="shared" si="1"/>
-        <v>0.34405594405594409</v>
-      </c>
-      <c r="G14" s="5">
-        <f t="shared" si="1"/>
-        <v>0.32027972027972029</v>
-      </c>
-      <c r="H14" s="5">
-        <f t="shared" si="1"/>
-        <v>0.38321678321678326</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="5">
-        <f t="shared" si="1"/>
-        <v>-3.5353535353535387E-2</v>
-      </c>
-      <c r="G15" s="5">
-        <f t="shared" si="1"/>
-        <v>-1.010101010101011E-3</v>
-      </c>
-      <c r="H15" s="5">
-        <f t="shared" si="1"/>
-        <v>4.0404040404040439E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="5">
-        <f>AVERAGE(F10:F15)</f>
-        <v>0.17320395038894273</v>
-      </c>
-      <c r="G16" s="5">
-        <f t="shared" ref="G16:H16" si="2">AVERAGE(G10:G15)</f>
-        <v>0.18392145165490137</v>
-      </c>
-      <c r="H16" s="5">
-        <f t="shared" si="2"/>
-        <v>0.21506560572966413</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C17" s="42"/>
       <c r="D17" s="42"/>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C18" s="42"/>
       <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C19" s="42"/>
       <c r="D19" s="42"/>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
       <c r="G19" s="42"/>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C20" s="42"/>
       <c r="D20" s="42"/>
       <c r="E20" s="42"/>
       <c r="F20" s="42"/>
       <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C3:C4"/>
+  <mergeCells count="9">
+    <mergeCell ref="J2:K2"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="C2:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
   </mergeCells>
-  <conditionalFormatting sqref="E3:H8">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="E5:K10">
+    <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
updated cot; correction results; need to rerun cot results with more tokens
</commit_message>
<xml_diff>
--- a/visualizations/join_results.xlsx
+++ b/visualizations/join_results.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/visualizations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A735C93B-EF65-EF46-8D7F-CDB31A6B868F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD76EA68-D631-EE4F-B00C-8023DE0EE367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="4880" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="4880" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="heuristics" sheetId="10" r:id="rId1"/>
     <sheet name="llm (hint)" sheetId="15" r:id="rId2"/>
     <sheet name="llm (values)" sheetId="14" r:id="rId3"/>
-    <sheet name="llm-correction" sheetId="9" r:id="rId4"/>
-    <sheet name="weak-ft" sheetId="8" r:id="rId5"/>
+    <sheet name="llm (cot)" sheetId="16" r:id="rId4"/>
+    <sheet name="llm-correction" sheetId="9" r:id="rId5"/>
+    <sheet name="weak-ft" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="62">
   <si>
     <t>4o-mini</t>
   </si>
@@ -201,9 +202,6 @@
 ($2.5/M)</t>
   </si>
   <si>
-    <t>No Fine-Tuning</t>
-  </si>
-  <si>
     <t>mistral (7b)</t>
   </si>
   <si>
@@ -226,6 +224,13 @@
   </si>
   <si>
     <t>4o</t>
+  </si>
+  <si>
+    <t>Few-
+Shot</t>
+  </si>
+  <si>
+    <t>models</t>
   </si>
 </sst>
 </file>
@@ -492,7 +497,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -707,150 +712,183 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -871,15 +909,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1240,7 +1269,7 @@
   <dimension ref="B2:AT51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R21" sqref="R21:T28"/>
+      <selection activeCell="AB38" sqref="AB38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -1282,49 +1311,49 @@
       <c r="F3" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="81"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="86"/>
       <c r="N3" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="80"/>
-      <c r="P3" s="80"/>
-      <c r="Q3" s="80"/>
-      <c r="R3" s="80"/>
-      <c r="S3" s="80"/>
-      <c r="T3" s="81"/>
-      <c r="U3" s="80" t="s">
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="85"/>
+      <c r="R3" s="85"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="86"/>
+      <c r="U3" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="V3" s="80"/>
-      <c r="W3" s="80"/>
-      <c r="X3" s="80"/>
-      <c r="Y3" s="81"/>
-      <c r="Z3" s="91" t="s">
+      <c r="V3" s="85"/>
+      <c r="W3" s="85"/>
+      <c r="X3" s="85"/>
+      <c r="Y3" s="86"/>
+      <c r="Z3" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="AA3" s="89"/>
-      <c r="AB3" s="89"/>
-      <c r="AC3" s="89"/>
-      <c r="AD3" s="90"/>
-      <c r="AE3" s="88" t="s">
+      <c r="AA3" s="98"/>
+      <c r="AB3" s="98"/>
+      <c r="AC3" s="98"/>
+      <c r="AD3" s="99"/>
+      <c r="AE3" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="AF3" s="89"/>
-      <c r="AG3" s="89"/>
-      <c r="AH3" s="89"/>
-      <c r="AI3" s="90"/>
-      <c r="AJ3" s="88" t="s">
+      <c r="AF3" s="98"/>
+      <c r="AG3" s="98"/>
+      <c r="AH3" s="98"/>
+      <c r="AI3" s="99"/>
+      <c r="AJ3" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="AK3" s="89"/>
-      <c r="AL3" s="89"/>
-      <c r="AM3" s="89"/>
-      <c r="AN3" s="90"/>
+      <c r="AK3" s="98"/>
+      <c r="AL3" s="98"/>
+      <c r="AM3" s="98"/>
+      <c r="AN3" s="99"/>
       <c r="AP3" s="18"/>
       <c r="AQ3" s="21" t="s">
         <v>18</v>
@@ -1340,7 +1369,7 @@
       </c>
     </row>
     <row r="4" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="81" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="21">
@@ -1349,52 +1378,52 @@
       <c r="D4" s="41">
         <v>0.86699999999999999</v>
       </c>
-      <c r="F4" s="85"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82" t="s">
+      <c r="F4" s="89"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="83"/>
-      <c r="N4" s="85"/>
-      <c r="O4" s="82"/>
-      <c r="P4" s="82" t="s">
+      <c r="I4" s="87"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="88"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="82"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="82"/>
-      <c r="T4" s="83"/>
-      <c r="U4" s="82" t="s">
+      <c r="Q4" s="87"/>
+      <c r="R4" s="87"/>
+      <c r="S4" s="87"/>
+      <c r="T4" s="88"/>
+      <c r="U4" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="V4" s="82"/>
-      <c r="W4" s="82"/>
-      <c r="X4" s="82"/>
-      <c r="Y4" s="83"/>
-      <c r="Z4" s="82" t="s">
+      <c r="V4" s="87"/>
+      <c r="W4" s="87"/>
+      <c r="X4" s="87"/>
+      <c r="Y4" s="88"/>
+      <c r="Z4" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="AA4" s="82"/>
-      <c r="AB4" s="82"/>
-      <c r="AC4" s="82"/>
-      <c r="AD4" s="83"/>
-      <c r="AE4" s="82" t="s">
+      <c r="AA4" s="87"/>
+      <c r="AB4" s="87"/>
+      <c r="AC4" s="87"/>
+      <c r="AD4" s="88"/>
+      <c r="AE4" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="AF4" s="82"/>
-      <c r="AG4" s="82"/>
-      <c r="AH4" s="82"/>
-      <c r="AI4" s="83"/>
-      <c r="AJ4" s="82" t="s">
+      <c r="AF4" s="87"/>
+      <c r="AG4" s="87"/>
+      <c r="AH4" s="87"/>
+      <c r="AI4" s="88"/>
+      <c r="AJ4" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="AK4" s="82"/>
-      <c r="AL4" s="82"/>
-      <c r="AM4" s="82"/>
-      <c r="AN4" s="83"/>
+      <c r="AK4" s="87"/>
+      <c r="AL4" s="87"/>
+      <c r="AM4" s="87"/>
+      <c r="AN4" s="88"/>
       <c r="AP4" s="29" t="s">
         <v>48</v>
       </c>
@@ -1416,15 +1445,15 @@
       </c>
     </row>
     <row r="5" spans="2:46" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="78"/>
+      <c r="B5" s="82"/>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="25">
         <v>0.90800000000000003</v>
       </c>
-      <c r="F5" s="86"/>
-      <c r="G5" s="87"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="91"/>
       <c r="H5" s="1">
         <v>1</v>
       </c>
@@ -1441,8 +1470,8 @@
         <v>5</v>
       </c>
       <c r="M5" s="24"/>
-      <c r="N5" s="86"/>
-      <c r="O5" s="87"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="91"/>
       <c r="P5" s="1">
         <v>1</v>
       </c>
@@ -1539,14 +1568,14 @@
       </c>
     </row>
     <row r="6" spans="2:46" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="78"/>
+      <c r="B6" s="82"/>
       <c r="C6" s="1">
         <v>5</v>
       </c>
       <c r="D6" s="25">
         <v>0.94599999999999995</v>
       </c>
-      <c r="F6" s="78" t="s">
+      <c r="F6" s="82" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="1">
@@ -1568,7 +1597,7 @@
         <v>0.83740632127728898</v>
       </c>
       <c r="M6" s="24"/>
-      <c r="N6" s="78" t="s">
+      <c r="N6" s="82" t="s">
         <v>4</v>
       </c>
       <c r="O6" s="1">
@@ -1670,14 +1699,14 @@
       </c>
     </row>
     <row r="7" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="78"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="1">
         <v>10</v>
       </c>
       <c r="D7" s="25">
         <v>0.94799999999999995</v>
       </c>
-      <c r="F7" s="78"/>
+      <c r="F7" s="82"/>
       <c r="G7" s="1">
         <v>2</v>
       </c>
@@ -1697,7 +1726,7 @@
         <v>0.88302400000000003</v>
       </c>
       <c r="M7" s="24"/>
-      <c r="N7" s="78"/>
+      <c r="N7" s="82"/>
       <c r="O7" s="1">
         <v>2</v>
       </c>
@@ -1778,14 +1807,14 @@
       </c>
     </row>
     <row r="8" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="79"/>
+      <c r="B8" s="83"/>
       <c r="C8" s="15">
         <v>20</v>
       </c>
       <c r="D8" s="27">
         <v>0.93400000000000005</v>
       </c>
-      <c r="F8" s="78"/>
+      <c r="F8" s="82"/>
       <c r="G8" s="1">
         <v>5</v>
       </c>
@@ -1805,7 +1834,7 @@
         <v>0.91756300000000002</v>
       </c>
       <c r="M8" s="24"/>
-      <c r="N8" s="78"/>
+      <c r="N8" s="82"/>
       <c r="O8" s="1">
         <v>5</v>
       </c>
@@ -1890,7 +1919,7 @@
       </c>
     </row>
     <row r="9" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B9" s="94" t="s">
+      <c r="B9" s="81" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="21">
@@ -1899,7 +1928,7 @@
       <c r="D9" s="41">
         <v>0.83799999999999997</v>
       </c>
-      <c r="F9" s="78"/>
+      <c r="F9" s="82"/>
       <c r="G9" s="1">
         <v>10</v>
       </c>
@@ -1919,7 +1948,7 @@
         <v>0.92538299999999996</v>
       </c>
       <c r="M9" s="24"/>
-      <c r="N9" s="78"/>
+      <c r="N9" s="82"/>
       <c r="O9" s="1">
         <v>10</v>
       </c>
@@ -2004,14 +2033,14 @@
       </c>
     </row>
     <row r="10" spans="2:46" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="78"/>
+      <c r="B10" s="82"/>
       <c r="C10" s="1">
         <v>2</v>
       </c>
       <c r="D10" s="25">
         <v>0.84699999999999998</v>
       </c>
-      <c r="F10" s="79"/>
+      <c r="F10" s="83"/>
       <c r="G10" s="15">
         <v>20</v>
       </c>
@@ -2031,7 +2060,7 @@
         <v>0.92049499999999995</v>
       </c>
       <c r="M10" s="24"/>
-      <c r="N10" s="79"/>
+      <c r="N10" s="83"/>
       <c r="O10" s="15">
         <v>20</v>
       </c>
@@ -2116,22 +2145,22 @@
       </c>
     </row>
     <row r="11" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="78"/>
+      <c r="B11" s="82"/>
       <c r="C11" s="1">
         <v>3</v>
       </c>
       <c r="D11" s="25">
         <v>0.85099999999999998</v>
       </c>
-      <c r="F11" s="85"/>
-      <c r="G11" s="82"/>
-      <c r="H11" s="82" t="s">
+      <c r="F11" s="89"/>
+      <c r="G11" s="87"/>
+      <c r="H11" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="82"/>
-      <c r="J11" s="82"/>
-      <c r="K11" s="82"/>
-      <c r="L11" s="83"/>
+      <c r="I11" s="87"/>
+      <c r="J11" s="87"/>
+      <c r="K11" s="87"/>
+      <c r="L11" s="88"/>
       <c r="M11" s="24"/>
       <c r="N11" s="42"/>
       <c r="P11" s="24"/>
@@ -2141,15 +2170,15 @@
       <c r="T11" s="24"/>
     </row>
     <row r="12" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="78"/>
+      <c r="B12" s="82"/>
       <c r="C12" s="1">
         <v>4</v>
       </c>
       <c r="D12" s="25">
         <v>0.85199999999999998</v>
       </c>
-      <c r="F12" s="86"/>
-      <c r="G12" s="87"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="91"/>
       <c r="H12" s="1">
         <v>0.1</v>
       </c>
@@ -2174,14 +2203,14 @@
       </c>
     </row>
     <row r="13" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="79"/>
+      <c r="B13" s="83"/>
       <c r="C13" s="15">
         <v>5</v>
       </c>
       <c r="D13" s="27">
         <v>0.83499999999999996</v>
       </c>
-      <c r="F13" s="78" t="s">
+      <c r="F13" s="82" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="1">
@@ -2204,7 +2233,7 @@
       </c>
     </row>
     <row r="14" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="94" t="s">
+      <c r="B14" s="81" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="21">
@@ -2213,7 +2242,7 @@
       <c r="D14" s="41">
         <v>0.65500000000000003</v>
       </c>
-      <c r="F14" s="78"/>
+      <c r="F14" s="82"/>
       <c r="G14" s="1">
         <v>2</v>
       </c>
@@ -2237,14 +2266,14 @@
       <c r="O14" s="24"/>
     </row>
     <row r="15" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B15" s="78"/>
+      <c r="B15" s="82"/>
       <c r="C15" s="1">
         <v>0.2</v>
       </c>
       <c r="D15" s="25">
         <v>0.70099999999999996</v>
       </c>
-      <c r="F15" s="78"/>
+      <c r="F15" s="82"/>
       <c r="G15" s="1">
         <v>5</v>
       </c>
@@ -2267,14 +2296,14 @@
       <c r="P15" s="5"/>
     </row>
     <row r="16" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B16" s="78"/>
+      <c r="B16" s="82"/>
       <c r="C16" s="1">
         <v>0.3</v>
       </c>
       <c r="D16" s="25">
         <v>0.73499999999999999</v>
       </c>
-      <c r="F16" s="78"/>
+      <c r="F16" s="82"/>
       <c r="G16" s="1">
         <v>10</v>
       </c>
@@ -2296,14 +2325,14 @@
       <c r="M16" s="24"/>
     </row>
     <row r="17" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="78"/>
+      <c r="B17" s="82"/>
       <c r="C17" s="1">
         <v>0.4</v>
       </c>
       <c r="D17" s="25">
         <v>0.753</v>
       </c>
-      <c r="F17" s="79"/>
+      <c r="F17" s="83"/>
       <c r="G17" s="15">
         <v>20</v>
       </c>
@@ -2330,22 +2359,22 @@
       <c r="T17" s="24"/>
     </row>
     <row r="18" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="79"/>
+      <c r="B18" s="83"/>
       <c r="C18" s="15">
         <v>0.5</v>
       </c>
       <c r="D18" s="27">
         <v>0.65400000000000003</v>
       </c>
-      <c r="F18" s="95"/>
-      <c r="G18" s="96"/>
-      <c r="H18" s="96" t="s">
+      <c r="F18" s="92"/>
+      <c r="G18" s="93"/>
+      <c r="H18" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="96"/>
-      <c r="J18" s="96"/>
-      <c r="K18" s="96"/>
-      <c r="L18" s="99"/>
+      <c r="I18" s="93"/>
+      <c r="J18" s="93"/>
+      <c r="K18" s="93"/>
+      <c r="L18" s="96"/>
       <c r="N18" s="42"/>
       <c r="P18" s="24"/>
       <c r="Q18" s="24"/>
@@ -2354,8 +2383,8 @@
       <c r="T18" s="24"/>
     </row>
     <row r="19" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F19" s="97"/>
-      <c r="G19" s="98"/>
+      <c r="F19" s="94"/>
+      <c r="G19" s="95"/>
       <c r="H19" s="1">
         <v>0.1</v>
       </c>
@@ -2379,7 +2408,7 @@
       <c r="T19" s="24"/>
     </row>
     <row r="20" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="92" t="s">
+      <c r="F20" s="79" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="44">
@@ -2403,7 +2432,7 @@
       <c r="P20" s="24"/>
     </row>
     <row r="21" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="92"/>
+      <c r="F21" s="79"/>
       <c r="G21" s="44">
         <v>2</v>
       </c>
@@ -2424,7 +2453,7 @@
       </c>
     </row>
     <row r="22" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F22" s="92"/>
+      <c r="F22" s="79"/>
       <c r="G22" s="44">
         <v>3</v>
       </c>
@@ -2446,7 +2475,7 @@
     </row>
     <row r="23" spans="2:40" x14ac:dyDescent="0.2">
       <c r="D23" s="42"/>
-      <c r="F23" s="92"/>
+      <c r="F23" s="79"/>
       <c r="G23" s="44">
         <v>4</v>
       </c>
@@ -2470,7 +2499,7 @@
     </row>
     <row r="24" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D24" s="42"/>
-      <c r="F24" s="93"/>
+      <c r="F24" s="80"/>
       <c r="G24" s="43">
         <v>5</v>
       </c>
@@ -2979,6 +3008,18 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="N6:N10"/>
+    <mergeCell ref="U3:Y3"/>
+    <mergeCell ref="U4:Y4"/>
+    <mergeCell ref="N3:T3"/>
+    <mergeCell ref="N4:O5"/>
+    <mergeCell ref="P4:T4"/>
+    <mergeCell ref="AJ3:AN3"/>
+    <mergeCell ref="AJ4:AN4"/>
+    <mergeCell ref="Z3:AD3"/>
+    <mergeCell ref="Z4:AD4"/>
+    <mergeCell ref="AE3:AI3"/>
+    <mergeCell ref="AE4:AI4"/>
     <mergeCell ref="F20:F24"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B14:B18"/>
@@ -2992,18 +3033,6 @@
     <mergeCell ref="F13:F17"/>
     <mergeCell ref="F18:G19"/>
     <mergeCell ref="H18:L18"/>
-    <mergeCell ref="AJ3:AN3"/>
-    <mergeCell ref="AJ4:AN4"/>
-    <mergeCell ref="Z3:AD3"/>
-    <mergeCell ref="Z4:AD4"/>
-    <mergeCell ref="AE3:AI3"/>
-    <mergeCell ref="AE4:AI4"/>
-    <mergeCell ref="N6:N10"/>
-    <mergeCell ref="U3:Y3"/>
-    <mergeCell ref="U4:Y4"/>
-    <mergeCell ref="N3:T3"/>
-    <mergeCell ref="N4:O5"/>
-    <mergeCell ref="P4:T4"/>
   </mergeCells>
   <conditionalFormatting sqref="D31:D43 P33:AD33 H33:L35 AJ33:AN35 P34:AC35 H38:L38 H39:H42 K39:L42 H45:L49">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -3059,7 +3088,7 @@
   <dimension ref="B1:W29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3080,31 +3109,31 @@
     <row r="1" spans="2:20" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B2" s="53"/>
-      <c r="D2" s="100" t="s">
+      <c r="D2" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="101" t="s">
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="101"/>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
-      <c r="L2" s="102"/>
+      <c r="I2" s="114"/>
+      <c r="J2" s="114"/>
+      <c r="K2" s="114"/>
+      <c r="L2" s="115"/>
     </row>
     <row r="3" spans="2:20" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="53"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="105"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="118"/>
       <c r="H3" s="59" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I3" s="59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J3" s="60" t="s">
         <v>50</v>
@@ -3120,193 +3149,191 @@
       <c r="B4" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="106" t="s">
+      <c r="D4" s="119" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="107"/>
-      <c r="F4" s="111" t="s">
+      <c r="E4" s="120"/>
+      <c r="F4" s="122" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="113">
+      <c r="H4" s="109">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="113"/>
-      <c r="J4" s="113"/>
-      <c r="K4" s="113"/>
-      <c r="L4" s="114"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="109"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="110"/>
     </row>
     <row r="5" spans="2:20" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="108"/>
-      <c r="E5" s="107"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="120"/>
       <c r="F5" s="112"/>
       <c r="G5" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="115">
+      <c r="H5" s="123">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="115"/>
-      <c r="J5" s="115"/>
-      <c r="K5" s="115"/>
-      <c r="L5" s="116"/>
+      <c r="I5" s="123"/>
+      <c r="J5" s="123"/>
+      <c r="K5" s="123"/>
+      <c r="L5" s="124"/>
     </row>
     <row r="6" spans="2:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="108"/>
-      <c r="E6" s="107"/>
-      <c r="F6" s="111" t="s">
+      <c r="D6" s="103"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="122" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="117">
+      <c r="H6" s="107">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="117"/>
-      <c r="J6" s="117"/>
-      <c r="K6" s="117"/>
-      <c r="L6" s="118"/>
+      <c r="I6" s="107"/>
+      <c r="J6" s="107"/>
+      <c r="K6" s="107"/>
+      <c r="L6" s="108"/>
     </row>
     <row r="7" spans="2:20" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="52"/>
-      <c r="D7" s="108"/>
-      <c r="E7" s="107"/>
+      <c r="D7" s="103"/>
+      <c r="E7" s="120"/>
       <c r="F7" s="112"/>
       <c r="G7" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="115">
+      <c r="H7" s="123">
         <v>0.85199999999999998</v>
       </c>
-      <c r="I7" s="115"/>
-      <c r="J7" s="115"/>
-      <c r="K7" s="115"/>
-      <c r="L7" s="116"/>
+      <c r="I7" s="123"/>
+      <c r="J7" s="123"/>
+      <c r="K7" s="123"/>
+      <c r="L7" s="124"/>
     </row>
     <row r="8" spans="2:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="53"/>
-      <c r="D8" s="108"/>
-      <c r="E8" s="107"/>
-      <c r="F8" s="111" t="s">
+      <c r="D8" s="103"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="122" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="117">
+      <c r="H8" s="107">
         <v>0.65400000000000003</v>
       </c>
-      <c r="I8" s="117"/>
-      <c r="J8" s="117"/>
-      <c r="K8" s="117"/>
-      <c r="L8" s="118"/>
+      <c r="I8" s="107"/>
+      <c r="J8" s="107"/>
+      <c r="K8" s="107"/>
+      <c r="L8" s="108"/>
     </row>
     <row r="9" spans="2:20" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="53"/>
-      <c r="D9" s="108"/>
-      <c r="E9" s="107"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="120"/>
       <c r="F9" s="112"/>
       <c r="G9" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="115">
+      <c r="H9" s="123">
         <v>0.753</v>
       </c>
-      <c r="I9" s="115"/>
-      <c r="J9" s="115"/>
-      <c r="K9" s="115"/>
-      <c r="L9" s="116"/>
+      <c r="I9" s="123"/>
+      <c r="J9" s="123"/>
+      <c r="K9" s="123"/>
+      <c r="L9" s="124"/>
     </row>
     <row r="10" spans="2:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="108"/>
-      <c r="E10" s="107"/>
-      <c r="F10" s="111" t="s">
+      <c r="D10" s="103"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="122" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="117">
+      <c r="H10" s="107">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I10" s="117"/>
-      <c r="J10" s="117"/>
-      <c r="K10" s="117"/>
-      <c r="L10" s="118"/>
+      <c r="I10" s="107"/>
+      <c r="J10" s="107"/>
+      <c r="K10" s="107"/>
+      <c r="L10" s="108"/>
     </row>
     <row r="11" spans="2:20" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="108"/>
-      <c r="E11" s="107"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="120"/>
       <c r="F11" s="112"/>
       <c r="G11" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="115">
+      <c r="H11" s="123">
         <v>0.98699999999999999</v>
       </c>
-      <c r="I11" s="115"/>
-      <c r="J11" s="115"/>
-      <c r="K11" s="115"/>
-      <c r="L11" s="116"/>
+      <c r="I11" s="123"/>
+      <c r="J11" s="123"/>
+      <c r="K11" s="123"/>
+      <c r="L11" s="124"/>
     </row>
     <row r="12" spans="2:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="108"/>
-      <c r="E12" s="107"/>
-      <c r="F12" s="111" t="s">
+      <c r="D12" s="103"/>
+      <c r="E12" s="120"/>
+      <c r="F12" s="122" t="s">
         <v>21</v>
       </c>
       <c r="G12" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="117">
+      <c r="H12" s="107">
         <v>0.71499999999999997</v>
       </c>
-      <c r="I12" s="117"/>
-      <c r="J12" s="117"/>
-      <c r="K12" s="117"/>
-      <c r="L12" s="118"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="107"/>
+      <c r="K12" s="107"/>
+      <c r="L12" s="108"/>
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
     <row r="13" spans="2:20" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="109"/>
-      <c r="E13" s="110"/>
-      <c r="F13" s="119"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="121"/>
+      <c r="F13" s="111"/>
       <c r="G13" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="113">
+      <c r="H13" s="109">
         <v>0.99</v>
       </c>
-      <c r="I13" s="113"/>
-      <c r="J13" s="113"/>
-      <c r="K13" s="113"/>
-      <c r="L13" s="114"/>
+      <c r="I13" s="109"/>
+      <c r="J13" s="109"/>
+      <c r="K13" s="109"/>
+      <c r="L13" s="110"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
     </row>
     <row r="14" spans="2:20" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="120" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="111" t="s">
+      <c r="D14" s="101" t="s">
         <v>1</v>
       </c>
+      <c r="E14" s="102"/>
       <c r="F14" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="81"/>
+      <c r="G14" s="86"/>
       <c r="H14" s="67">
         <v>0.52</v>
       </c>
@@ -3345,9 +3372,9 @@
       </c>
     </row>
     <row r="15" spans="2:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="108"/>
-      <c r="E15" s="119"/>
-      <c r="F15" s="119" t="s">
+      <c r="D15" s="103"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="111" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -3391,9 +3418,9 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D16" s="108"/>
-      <c r="E16" s="119"/>
-      <c r="F16" s="119"/>
+      <c r="D16" s="103"/>
+      <c r="E16" s="104"/>
+      <c r="F16" s="111"/>
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
@@ -3419,9 +3446,9 @@
       <c r="S16" s="31"/>
     </row>
     <row r="17" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D17" s="108"/>
-      <c r="E17" s="119"/>
-      <c r="F17" s="119"/>
+      <c r="D17" s="103"/>
+      <c r="E17" s="104"/>
+      <c r="F17" s="111"/>
       <c r="G17" s="1" t="s">
         <v>22</v>
       </c>
@@ -3448,9 +3475,9 @@
       <c r="W17" s="5"/>
     </row>
     <row r="18" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D18" s="108"/>
-      <c r="E18" s="119"/>
-      <c r="F18" s="119"/>
+      <c r="D18" s="103"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="111"/>
       <c r="G18" s="1" t="s">
         <v>45</v>
       </c>
@@ -3476,9 +3503,9 @@
       <c r="S18" s="31"/>
     </row>
     <row r="19" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D19" s="108"/>
-      <c r="E19" s="119"/>
-      <c r="F19" s="119"/>
+      <c r="D19" s="103"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="111"/>
       <c r="G19" s="1" t="s">
         <v>46</v>
       </c>
@@ -3504,9 +3531,9 @@
       <c r="S19" s="31"/>
     </row>
     <row r="20" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D20" s="108"/>
-      <c r="E20" s="119"/>
-      <c r="F20" s="119"/>
+      <c r="D20" s="103"/>
+      <c r="E20" s="104"/>
+      <c r="F20" s="111"/>
       <c r="G20" s="1" t="s">
         <v>47</v>
       </c>
@@ -3532,8 +3559,8 @@
       <c r="S20" s="31"/>
     </row>
     <row r="21" spans="4:23" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="108"/>
-      <c r="E21" s="119"/>
+      <c r="D21" s="103"/>
+      <c r="E21" s="104"/>
       <c r="F21" s="112"/>
       <c r="G21" s="15" t="s">
         <v>21</v>
@@ -3560,14 +3587,14 @@
       <c r="S21" s="31"/>
     </row>
     <row r="22" spans="4:23" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="108"/>
-      <c r="E22" s="111" t="s">
+      <c r="D22" s="103" t="s">
         <v>2</v>
       </c>
+      <c r="E22" s="104"/>
       <c r="F22" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="81"/>
+      <c r="G22" s="86"/>
       <c r="H22" s="68">
         <v>0.495</v>
       </c>
@@ -3590,9 +3617,9 @@
       <c r="S22" s="31"/>
     </row>
     <row r="23" spans="4:23" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="108"/>
-      <c r="E23" s="119"/>
-      <c r="F23" s="119" t="s">
+      <c r="D23" s="103"/>
+      <c r="E23" s="104"/>
+      <c r="F23" s="111" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -3620,9 +3647,9 @@
       <c r="S23" s="31"/>
     </row>
     <row r="24" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D24" s="108"/>
-      <c r="E24" s="119"/>
-      <c r="F24" s="119"/>
+      <c r="D24" s="103"/>
+      <c r="E24" s="104"/>
+      <c r="F24" s="111"/>
       <c r="G24" s="1" t="s">
         <v>12</v>
       </c>
@@ -3648,9 +3675,9 @@
       <c r="S24" s="31"/>
     </row>
     <row r="25" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D25" s="108"/>
-      <c r="E25" s="119"/>
-      <c r="F25" s="119"/>
+      <c r="D25" s="103"/>
+      <c r="E25" s="104"/>
+      <c r="F25" s="111"/>
       <c r="G25" s="1" t="s">
         <v>22</v>
       </c>
@@ -3676,9 +3703,9 @@
       <c r="S25" s="31"/>
     </row>
     <row r="26" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D26" s="108"/>
-      <c r="E26" s="119"/>
-      <c r="F26" s="119"/>
+      <c r="D26" s="103"/>
+      <c r="E26" s="104"/>
+      <c r="F26" s="111"/>
       <c r="G26" s="1" t="s">
         <v>45</v>
       </c>
@@ -3704,9 +3731,9 @@
       <c r="S26" s="31"/>
     </row>
     <row r="27" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D27" s="108"/>
-      <c r="E27" s="119"/>
-      <c r="F27" s="119"/>
+      <c r="D27" s="103"/>
+      <c r="E27" s="104"/>
+      <c r="F27" s="111"/>
       <c r="G27" s="1" t="s">
         <v>46</v>
       </c>
@@ -3732,9 +3759,9 @@
       <c r="S27" s="31"/>
     </row>
     <row r="28" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D28" s="108"/>
-      <c r="E28" s="119"/>
-      <c r="F28" s="119"/>
+      <c r="D28" s="103"/>
+      <c r="E28" s="104"/>
+      <c r="F28" s="111"/>
       <c r="G28" s="1" t="s">
         <v>47</v>
       </c>
@@ -3760,8 +3787,8 @@
       <c r="S28" s="31"/>
     </row>
     <row r="29" spans="4:23" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="109"/>
-      <c r="E29" s="112"/>
+      <c r="D29" s="105"/>
+      <c r="E29" s="106"/>
       <c r="F29" s="112"/>
       <c r="G29" s="15" t="s">
         <v>21</v>
@@ -3788,16 +3815,7 @@
       <c r="S29" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="D14:D29"/>
-    <mergeCell ref="E14:E21"/>
-    <mergeCell ref="F15:F21"/>
-    <mergeCell ref="E22:E29"/>
-    <mergeCell ref="F23:F29"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F22:G22"/>
+  <mergeCells count="24">
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D4:E13"/>
@@ -3814,6 +3832,14 @@
     <mergeCell ref="H10:L10"/>
     <mergeCell ref="H11:L11"/>
     <mergeCell ref="F12:F13"/>
+    <mergeCell ref="D14:E21"/>
+    <mergeCell ref="D22:E29"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="F15:F21"/>
+    <mergeCell ref="F23:F29"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F22:G22"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:L29">
     <cfRule type="colorScale" priority="52">
@@ -3837,7 +3863,7 @@
   <dimension ref="B1:U27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3858,31 +3884,31 @@
     <row r="1" spans="2:21" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B2" s="53"/>
-      <c r="D2" s="100" t="s">
+      <c r="D2" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="101" t="s">
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="101"/>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
-      <c r="L2" s="102"/>
+      <c r="I2" s="114"/>
+      <c r="J2" s="114"/>
+      <c r="K2" s="114"/>
+      <c r="L2" s="115"/>
     </row>
     <row r="3" spans="2:21" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="53"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="105"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="118"/>
       <c r="H3" s="59" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I3" s="59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J3" s="60" t="s">
         <v>50</v>
@@ -3898,184 +3924,182 @@
       <c r="B4" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="106" t="s">
+      <c r="D4" s="119" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="107"/>
-      <c r="F4" s="111" t="s">
+      <c r="E4" s="120"/>
+      <c r="F4" s="122" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="113">
+      <c r="H4" s="125">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="113"/>
-      <c r="J4" s="113"/>
-      <c r="K4" s="113"/>
-      <c r="L4" s="114"/>
+      <c r="I4" s="107"/>
+      <c r="J4" s="107"/>
+      <c r="K4" s="107"/>
+      <c r="L4" s="108"/>
     </row>
     <row r="5" spans="2:21" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="108"/>
-      <c r="E5" s="107"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="120"/>
       <c r="F5" s="112"/>
       <c r="G5" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="115">
+      <c r="H5" s="126">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="115"/>
-      <c r="J5" s="115"/>
-      <c r="K5" s="115"/>
-      <c r="L5" s="116"/>
+      <c r="I5" s="123"/>
+      <c r="J5" s="123"/>
+      <c r="K5" s="123"/>
+      <c r="L5" s="124"/>
     </row>
     <row r="6" spans="2:21" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="108"/>
-      <c r="E6" s="107"/>
-      <c r="F6" s="111" t="s">
+      <c r="D6" s="103"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="122" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="117">
+      <c r="H6" s="107">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="117"/>
-      <c r="J6" s="117"/>
-      <c r="K6" s="117"/>
-      <c r="L6" s="118"/>
+      <c r="I6" s="107"/>
+      <c r="J6" s="107"/>
+      <c r="K6" s="107"/>
+      <c r="L6" s="108"/>
     </row>
     <row r="7" spans="2:21" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="52"/>
-      <c r="D7" s="108"/>
-      <c r="E7" s="107"/>
+      <c r="D7" s="103"/>
+      <c r="E7" s="120"/>
       <c r="F7" s="112"/>
       <c r="G7" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="115">
+      <c r="H7" s="123">
         <v>0.85199999999999998</v>
       </c>
-      <c r="I7" s="115"/>
-      <c r="J7" s="115"/>
-      <c r="K7" s="115"/>
-      <c r="L7" s="116"/>
+      <c r="I7" s="123"/>
+      <c r="J7" s="123"/>
+      <c r="K7" s="123"/>
+      <c r="L7" s="124"/>
     </row>
     <row r="8" spans="2:21" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="53"/>
-      <c r="D8" s="108"/>
-      <c r="E8" s="107"/>
-      <c r="F8" s="111" t="s">
+      <c r="D8" s="103"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="122" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="117">
+      <c r="H8" s="107">
         <v>0.65400000000000003</v>
       </c>
-      <c r="I8" s="117"/>
-      <c r="J8" s="117"/>
-      <c r="K8" s="117"/>
-      <c r="L8" s="118"/>
+      <c r="I8" s="107"/>
+      <c r="J8" s="107"/>
+      <c r="K8" s="107"/>
+      <c r="L8" s="108"/>
     </row>
     <row r="9" spans="2:21" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="53"/>
-      <c r="D9" s="108"/>
-      <c r="E9" s="107"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="120"/>
       <c r="F9" s="112"/>
       <c r="G9" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="115">
+      <c r="H9" s="123">
         <v>0.753</v>
       </c>
-      <c r="I9" s="115"/>
-      <c r="J9" s="115"/>
-      <c r="K9" s="115"/>
-      <c r="L9" s="116"/>
+      <c r="I9" s="123"/>
+      <c r="J9" s="123"/>
+      <c r="K9" s="123"/>
+      <c r="L9" s="124"/>
     </row>
     <row r="10" spans="2:21" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="108"/>
-      <c r="E10" s="107"/>
-      <c r="F10" s="111" t="s">
+      <c r="D10" s="103"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="122" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="117">
+      <c r="H10" s="107">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I10" s="117"/>
-      <c r="J10" s="117"/>
-      <c r="K10" s="117"/>
-      <c r="L10" s="118"/>
+      <c r="I10" s="107"/>
+      <c r="J10" s="107"/>
+      <c r="K10" s="107"/>
+      <c r="L10" s="108"/>
     </row>
     <row r="11" spans="2:21" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="108"/>
-      <c r="E11" s="107"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="120"/>
       <c r="F11" s="112"/>
       <c r="G11" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="115">
+      <c r="H11" s="123">
         <v>0.98699999999999999</v>
       </c>
-      <c r="I11" s="115"/>
-      <c r="J11" s="115"/>
-      <c r="K11" s="115"/>
-      <c r="L11" s="116"/>
+      <c r="I11" s="123"/>
+      <c r="J11" s="123"/>
+      <c r="K11" s="123"/>
+      <c r="L11" s="124"/>
     </row>
     <row r="12" spans="2:21" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="108"/>
-      <c r="E12" s="107"/>
-      <c r="F12" s="111" t="s">
+      <c r="D12" s="103"/>
+      <c r="E12" s="120"/>
+      <c r="F12" s="122" t="s">
         <v>21</v>
       </c>
       <c r="G12" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="117">
+      <c r="H12" s="107">
         <v>0.71499999999999997</v>
       </c>
-      <c r="I12" s="117"/>
-      <c r="J12" s="117"/>
-      <c r="K12" s="117"/>
-      <c r="L12" s="118"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="107"/>
+      <c r="K12" s="107"/>
+      <c r="L12" s="108"/>
     </row>
     <row r="13" spans="2:21" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="109"/>
-      <c r="E13" s="110"/>
-      <c r="F13" s="119"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="121"/>
+      <c r="F13" s="111"/>
       <c r="G13" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="113">
+      <c r="H13" s="109">
         <v>0.99</v>
       </c>
-      <c r="I13" s="113"/>
-      <c r="J13" s="113"/>
-      <c r="K13" s="113"/>
-      <c r="L13" s="114"/>
+      <c r="I13" s="109"/>
+      <c r="J13" s="109"/>
+      <c r="K13" s="109"/>
+      <c r="L13" s="110"/>
     </row>
     <row r="14" spans="2:21" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="111" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="108" t="s">
+      <c r="D14" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="111" t="s">
+      <c r="E14" s="102"/>
+      <c r="F14" s="122" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="21" t="s">
@@ -4119,9 +4143,9 @@
       <c r="U14" s="5"/>
     </row>
     <row r="15" spans="2:21" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="119"/>
-      <c r="E15" s="108"/>
-      <c r="F15" s="119"/>
+      <c r="D15" s="103"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="111"/>
       <c r="G15" s="1" t="s">
         <v>12</v>
       </c>
@@ -4163,9 +4187,9 @@
       <c r="U15" s="5"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="D16" s="119"/>
-      <c r="E16" s="108"/>
-      <c r="F16" s="119"/>
+      <c r="D16" s="103"/>
+      <c r="E16" s="104"/>
+      <c r="F16" s="111"/>
       <c r="G16" s="1" t="s">
         <v>22</v>
       </c>
@@ -4186,9 +4210,9 @@
       </c>
     </row>
     <row r="17" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D17" s="119"/>
-      <c r="E17" s="108"/>
-      <c r="F17" s="119"/>
+      <c r="D17" s="103"/>
+      <c r="E17" s="104"/>
+      <c r="F17" s="111"/>
       <c r="G17" s="1" t="s">
         <v>45</v>
       </c>
@@ -4214,9 +4238,9 @@
       <c r="U17" s="5"/>
     </row>
     <row r="18" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D18" s="119"/>
-      <c r="E18" s="108"/>
-      <c r="F18" s="119"/>
+      <c r="D18" s="103"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="111"/>
       <c r="G18" s="1" t="s">
         <v>46</v>
       </c>
@@ -4237,9 +4261,9 @@
       </c>
     </row>
     <row r="19" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D19" s="119"/>
-      <c r="E19" s="108"/>
-      <c r="F19" s="119"/>
+      <c r="D19" s="103"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="111"/>
       <c r="G19" s="1" t="s">
         <v>47</v>
       </c>
@@ -4263,8 +4287,8 @@
       <c r="Q19" s="5"/>
     </row>
     <row r="20" spans="4:21" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="119"/>
-      <c r="E20" s="109"/>
+      <c r="D20" s="103"/>
+      <c r="E20" s="104"/>
       <c r="F20" s="112"/>
       <c r="G20" s="15" t="s">
         <v>21</v>
@@ -4285,12 +4309,12 @@
         <v>0.86099999999999999</v>
       </c>
     </row>
-    <row r="21" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D21" s="119"/>
-      <c r="E21" s="111" t="s">
+    <row r="21" spans="4:21" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="111" t="s">
+      <c r="E21" s="104"/>
+      <c r="F21" s="122" t="s">
         <v>10</v>
       </c>
       <c r="G21" s="1" t="s">
@@ -4313,9 +4337,9 @@
       </c>
     </row>
     <row r="22" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D22" s="119"/>
-      <c r="E22" s="119"/>
-      <c r="F22" s="119"/>
+      <c r="D22" s="103"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="111"/>
       <c r="G22" s="1" t="s">
         <v>12</v>
       </c>
@@ -4336,9 +4360,9 @@
       </c>
     </row>
     <row r="23" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D23" s="119"/>
-      <c r="E23" s="119"/>
-      <c r="F23" s="119"/>
+      <c r="D23" s="103"/>
+      <c r="E23" s="104"/>
+      <c r="F23" s="111"/>
       <c r="G23" s="1" t="s">
         <v>22</v>
       </c>
@@ -4359,9 +4383,9 @@
       </c>
     </row>
     <row r="24" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D24" s="119"/>
-      <c r="E24" s="119"/>
-      <c r="F24" s="119"/>
+      <c r="D24" s="103"/>
+      <c r="E24" s="104"/>
+      <c r="F24" s="111"/>
       <c r="G24" s="1" t="s">
         <v>45</v>
       </c>
@@ -4382,9 +4406,9 @@
       </c>
     </row>
     <row r="25" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D25" s="119"/>
-      <c r="E25" s="119"/>
-      <c r="F25" s="119"/>
+      <c r="D25" s="103"/>
+      <c r="E25" s="104"/>
+      <c r="F25" s="111"/>
       <c r="G25" s="1" t="s">
         <v>46</v>
       </c>
@@ -4405,9 +4429,9 @@
       </c>
     </row>
     <row r="26" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D26" s="119"/>
-      <c r="E26" s="119"/>
-      <c r="F26" s="119"/>
+      <c r="D26" s="103"/>
+      <c r="E26" s="104"/>
+      <c r="F26" s="111"/>
       <c r="G26" s="1" t="s">
         <v>47</v>
       </c>
@@ -4428,8 +4452,8 @@
       </c>
     </row>
     <row r="27" spans="4:21" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="112"/>
-      <c r="E27" s="112"/>
+      <c r="D27" s="105"/>
+      <c r="E27" s="106"/>
       <c r="F27" s="112"/>
       <c r="G27" s="15" t="s">
         <v>21</v>
@@ -4451,7 +4475,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="22">
+    <mergeCell ref="H10:L10"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="F14:F20"/>
+    <mergeCell ref="F21:F27"/>
+    <mergeCell ref="D14:E20"/>
+    <mergeCell ref="D21:E27"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D4:E13"/>
@@ -4468,13 +4498,6 @@
     <mergeCell ref="H12:L12"/>
     <mergeCell ref="H13:L13"/>
     <mergeCell ref="F10:F11"/>
-    <mergeCell ref="H10:L10"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="D14:D27"/>
-    <mergeCell ref="E14:E20"/>
-    <mergeCell ref="F14:F20"/>
-    <mergeCell ref="E21:E27"/>
-    <mergeCell ref="F21:F27"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:L27">
     <cfRule type="colorScale" priority="55">
@@ -4494,327 +4517,272 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D718D1-05D9-2146-B7ED-D601D310FD08}">
-  <dimension ref="B1:K22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F339B4-372A-B44E-B41D-D416A194057A}">
+  <dimension ref="B1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="6" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="3"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-    </row>
-    <row r="2" spans="2:11" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="123"/>
-      <c r="D2" s="124"/>
-      <c r="E2" s="121" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="128" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="129"/>
-      <c r="H2" s="128" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" s="129"/>
-      <c r="J2" s="130" t="s">
+    <row r="1" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B2" s="53"/>
+      <c r="D2" s="113" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="114" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="114"/>
+      <c r="J2" s="115"/>
+    </row>
+    <row r="3" spans="2:14" ht="41" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="53"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="61" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="119" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="120"/>
+      <c r="F4" s="122" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="63" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="125">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="I4" s="107"/>
+      <c r="J4" s="108"/>
+    </row>
+    <row r="5" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="103"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="126">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="I5" s="123"/>
+      <c r="J5" s="124"/>
+    </row>
+    <row r="6" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="103"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="122" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="125">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="I6" s="107"/>
+      <c r="J6" s="108"/>
+    </row>
+    <row r="7" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="52"/>
+      <c r="D7" s="103"/>
+      <c r="E7" s="120"/>
+      <c r="F7" s="112"/>
+      <c r="G7" s="64" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="126">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="I7" s="123"/>
+      <c r="J7" s="124"/>
+    </row>
+    <row r="8" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="53"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="122" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="125">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="I8" s="107"/>
+      <c r="J8" s="108"/>
+    </row>
+    <row r="9" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="53"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="120"/>
+      <c r="F9" s="112"/>
+      <c r="G9" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="126">
+        <v>0.753</v>
+      </c>
+      <c r="I9" s="123"/>
+      <c r="J9" s="124"/>
+    </row>
+    <row r="10" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="103"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="122" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="65" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="125">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="I10" s="107"/>
+      <c r="J10" s="108"/>
+    </row>
+    <row r="11" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="103"/>
+      <c r="E11" s="120"/>
+      <c r="F11" s="112"/>
+      <c r="G11" s="66" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="126">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="I11" s="123"/>
+      <c r="J11" s="124"/>
+    </row>
+    <row r="12" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="103"/>
+      <c r="E12" s="120"/>
+      <c r="F12" s="122" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="125">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="I12" s="107"/>
+      <c r="J12" s="108"/>
+    </row>
+    <row r="13" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="105"/>
+      <c r="E13" s="121"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="126">
+        <v>0.99</v>
+      </c>
+      <c r="I13" s="123"/>
+      <c r="J13" s="124"/>
+    </row>
+    <row r="14" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="127" t="s">
         <v>60</v>
       </c>
-      <c r="K2" s="129"/>
-    </row>
-    <row r="3" spans="2:11" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="125"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="70" t="s">
+      <c r="E14" s="128"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="55"/>
+      <c r="N14" s="5"/>
+    </row>
+    <row r="15" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="103"/>
+      <c r="E15" s="120"/>
+      <c r="F15" s="104"/>
+      <c r="G15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="14"/>
+      <c r="N15" s="5"/>
+    </row>
+    <row r="16" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="105"/>
+      <c r="E16" s="121"/>
+      <c r="F16" s="106"/>
+      <c r="G16" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="71" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="I3" s="71" t="s">
-        <v>56</v>
-      </c>
-      <c r="J3" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="K3" s="71" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C4" s="123" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="127"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="71"/>
-    </row>
-    <row r="5" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="86" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="75">
-        <v>0.65400000000000003</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="23">
-        <v>0.94499999999999995</v>
-      </c>
-      <c r="I5" s="23">
-        <v>0.95699999999999996</v>
-      </c>
-      <c r="K5" s="23">
-        <v>0.99199999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="86"/>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="75">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="23">
-        <v>0.96599999999999997</v>
-      </c>
-      <c r="I6" s="23">
-        <v>0.97399999999999998</v>
-      </c>
-      <c r="K6" s="23">
-        <v>0.97599999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="86" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="75">
-        <v>0.73499999999999999</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="23">
-        <v>0.95699999999999996</v>
-      </c>
-      <c r="I7" s="13">
-        <v>0.95</v>
-      </c>
-      <c r="J7" s="5"/>
-      <c r="K7" s="23">
-        <v>0.995</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C8" s="86"/>
-      <c r="D8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="75">
-        <v>0.98699999999999999</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="23">
-        <v>0.95199999999999996</v>
-      </c>
-      <c r="I8" s="23">
-        <v>0.98799999999999999</v>
-      </c>
-      <c r="K8" s="13">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="86" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="76">
-        <v>0.71499999999999997</v>
-      </c>
-      <c r="F9" s="45"/>
-      <c r="G9" s="23">
-        <v>0.96099999999999997</v>
-      </c>
-      <c r="I9" s="23">
-        <v>0.94399999999999995</v>
-      </c>
-      <c r="K9" s="23">
-        <v>0.98899999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="131"/>
-      <c r="D10" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="77">
-        <v>0.99</v>
-      </c>
-      <c r="F10" s="73"/>
-      <c r="G10" s="66">
-        <v>0.95499999999999996</v>
-      </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="66">
-        <v>0.98899999999999999</v>
-      </c>
-      <c r="J10" s="15"/>
-      <c r="K10" s="66">
-        <v>0.99399999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
-    </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-    </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-    </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="C2:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
+  <mergeCells count="19">
+    <mergeCell ref="D14:F16"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="D4:E13"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="F8:F9"/>
   </mergeCells>
-  <conditionalFormatting sqref="E5:K10">
-    <cfRule type="colorScale" priority="58">
+  <conditionalFormatting sqref="H4:J16">
+    <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4831,6 +4799,396 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D718D1-05D9-2146-B7ED-D601D310FD08}">
+  <dimension ref="B1:K22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="3"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="2:11" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="134"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="132" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="139" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="130"/>
+      <c r="H2" s="139" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="130"/>
+      <c r="J2" s="129" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" s="130"/>
+    </row>
+    <row r="3" spans="2:11" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="136"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="133"/>
+      <c r="F3" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" s="71" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C4" s="134" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="138"/>
+      <c r="E4" s="78">
+        <v>0.501</v>
+      </c>
+      <c r="F4" s="77">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="G4" s="65"/>
+      <c r="H4" s="77">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="I4" s="65"/>
+      <c r="J4" s="77">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="K4" s="65"/>
+    </row>
+    <row r="5" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="90" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="74">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.41</v>
+      </c>
+      <c r="G5" s="23">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="I5" s="13">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0.628</v>
+      </c>
+      <c r="K5" s="23">
+        <v>0.99199999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="90"/>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="74">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="G6" s="23">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="I6" s="13">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="K6" s="23">
+        <v>0.97599999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="90" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="74">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="G7" s="23">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="I7" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="K7" s="23">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C8" s="90"/>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="74">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.378</v>
+      </c>
+      <c r="G8" s="23">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="I8" s="13">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="K8" s="13">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="90" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="75">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="F9" s="45">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="G9" s="23">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="I9" s="13">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="K9" s="23">
+        <v>0.98899999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="131"/>
+      <c r="D10" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="76">
+        <v>0.99</v>
+      </c>
+      <c r="F10" s="73">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="G10" s="66">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="H10" s="19">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="I10" s="20">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="J10" s="19">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="K10" s="66">
+        <v>0.99399999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="C2:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E4:K10">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color theme="6" tint="-0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D01CA2-3159-F448-9006-FF836418E31D}">
   <dimension ref="A1:H52"/>
   <sheetViews>

</xml_diff>

<commit_message>
updated cot & correction results; good
</commit_message>
<xml_diff>
--- a/visualizations/join_results.xlsx
+++ b/visualizations/join_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/visualizations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD76EA68-D631-EE4F-B00C-8023DE0EE367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4AD315-474E-C64B-81BF-F2379F030D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="4880" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="4880" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="heuristics" sheetId="10" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="68">
   <si>
     <t>4o-mini</t>
   </si>
@@ -231,6 +231,24 @@
   </si>
   <si>
     <t>models</t>
+  </si>
+  <si>
+    <t>worst single</t>
+  </si>
+  <si>
+    <t>best single</t>
+  </si>
+  <si>
+    <t>worst duo</t>
+  </si>
+  <si>
+    <t>best duo</t>
+  </si>
+  <si>
+    <t>worst trio</t>
+  </si>
+  <si>
+    <t>best trio</t>
   </si>
 </sst>
 </file>
@@ -497,7 +515,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -883,9 +901,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -904,11 +919,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1269,7 +1290,7 @@
   <dimension ref="B2:AT51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AB38" sqref="AB38"/>
+      <selection activeCell="Y23" sqref="Y23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2689,7 +2710,6 @@
       <c r="M33" s="24"/>
       <c r="N33" s="56"/>
       <c r="P33" s="24"/>
-      <c r="Q33" s="24"/>
       <c r="R33" s="24"/>
       <c r="S33" s="24"/>
       <c r="T33" s="24"/>
@@ -2726,7 +2746,6 @@
       <c r="M34" s="24"/>
       <c r="N34" s="56"/>
       <c r="P34" s="37"/>
-      <c r="Q34" s="37"/>
       <c r="R34" s="37"/>
       <c r="S34" s="37"/>
       <c r="T34" s="37"/>
@@ -2763,7 +2782,6 @@
       <c r="M35" s="24"/>
       <c r="N35" s="56"/>
       <c r="P35" s="37"/>
-      <c r="Q35" s="37"/>
       <c r="R35" s="37"/>
       <c r="S35" s="37"/>
       <c r="T35" s="37"/>
@@ -3034,7 +3052,7 @@
     <mergeCell ref="F18:G19"/>
     <mergeCell ref="H18:L18"/>
   </mergeCells>
-  <conditionalFormatting sqref="D31:D43 P33:AD33 H33:L35 AJ33:AN35 P34:AC35 H38:L38 H39:H42 K39:L42 H45:L49">
+  <conditionalFormatting sqref="D31:D43 R33:AD33 H33:L35 P33:P35 AJ33:AN35 R34:AC35 H38:L38 H39:H42 K39:L42 H45:L49">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0.969</formula>
     </cfRule>
@@ -3088,7 +3106,7 @@
   <dimension ref="B1:W29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+      <selection activeCell="J29" activeCellId="1" sqref="J22:K22 J29:K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3307,7 +3325,7 @@
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="2:20" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:20" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="105"/>
       <c r="E13" s="121"/>
       <c r="F13" s="111"/>
@@ -3321,9 +3339,11 @@
       <c r="J13" s="109"/>
       <c r="K13" s="109"/>
       <c r="L13" s="110"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
+      <c r="P13" s="72"/>
+      <c r="Q13" s="72"/>
+      <c r="R13" s="72"/>
+      <c r="S13" s="72"/>
+      <c r="T13" s="72"/>
     </row>
     <row r="14" spans="2:20" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="101" t="s">
@@ -3525,9 +3545,9 @@
         <v>0.41299999999999998</v>
       </c>
       <c r="O19" s="31"/>
-      <c r="P19" s="31"/>
+      <c r="P19" s="72"/>
       <c r="Q19" s="31"/>
-      <c r="R19" s="31"/>
+      <c r="R19" s="72"/>
       <c r="S19" s="31"/>
     </row>
     <row r="20" spans="4:23" x14ac:dyDescent="0.25">
@@ -3642,9 +3662,15 @@
       </c>
       <c r="O23" s="31"/>
       <c r="P23" s="31"/>
-      <c r="Q23" s="31"/>
+      <c r="Q23" s="72">
+        <f>AVERAGE(H14:L21)</f>
+        <v>0.541825</v>
+      </c>
       <c r="R23" s="31"/>
-      <c r="S23" s="31"/>
+      <c r="S23" s="72">
+        <f>(0.9-Q23)/0.9</f>
+        <v>0.39797222222222223</v>
+      </c>
     </row>
     <row r="24" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D24" s="103"/>
@@ -3670,9 +3696,15 @@
       </c>
       <c r="O24" s="31"/>
       <c r="P24" s="31"/>
-      <c r="Q24" s="31"/>
+      <c r="Q24" s="72">
+        <f>AVERAGE(H22:L29)</f>
+        <v>0.57537500000000008</v>
+      </c>
       <c r="R24" s="31"/>
-      <c r="S24" s="31"/>
+      <c r="S24" s="72">
+        <f>(0.9-Q24)/0.9</f>
+        <v>0.36069444444444437</v>
+      </c>
     </row>
     <row r="25" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D25" s="103"/>
@@ -3863,7 +3895,7 @@
   <dimension ref="B1:U27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="J27" sqref="J27:K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -4518,10 +4550,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F339B4-372A-B44E-B41D-D416A194057A}">
-  <dimension ref="B1:N16"/>
+  <dimension ref="B1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -4731,8 +4763,12 @@
       <c r="G14" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
+      <c r="H14" s="54">
+        <v>0.46</v>
+      </c>
+      <c r="I14" s="54">
+        <v>0.67300000000000004</v>
+      </c>
       <c r="J14" s="55"/>
       <c r="N14" s="5"/>
     </row>
@@ -4743,8 +4779,12 @@
       <c r="G15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="H15" s="6">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0.76</v>
+      </c>
       <c r="J15" s="14"/>
       <c r="N15" s="5"/>
     </row>
@@ -4755,9 +4795,37 @@
       <c r="G16" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
+      <c r="H16" s="16">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="I16" s="16">
+        <v>0.98099999999999998</v>
+      </c>
       <c r="J16" s="17"/>
+    </row>
+    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H19" s="6">
+        <v>0.495</v>
+      </c>
+      <c r="I19" s="6">
+        <v>0.63300000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="8:9" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H20" s="16">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="I20" s="16">
+        <v>0.65300000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="8:9" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="16">
+        <v>0.872</v>
+      </c>
+      <c r="I21" s="16">
+        <v>0.98399999999999999</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="19">
@@ -4782,7 +4850,31 @@
     <mergeCell ref="F8:F9"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:J16">
-    <cfRule type="colorScale" priority="62">
+    <cfRule type="colorScale" priority="64">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color theme="6" tint="-0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19:I20">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color theme="6" tint="-0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21:I21">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4800,10 +4892,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D718D1-05D9-2146-B7ED-D601D310FD08}">
-  <dimension ref="B1:K22"/>
+  <dimension ref="B1:AB22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -4822,7 +4914,7 @@
     <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:28" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -4833,17 +4925,17 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="2:11" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="134"/>
-      <c r="D2" s="135"/>
-      <c r="E2" s="132" t="s">
+    <row r="2" spans="2:28" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="133"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="139" t="s">
+      <c r="F2" s="137" t="s">
         <v>57</v>
       </c>
       <c r="G2" s="130"/>
-      <c r="H2" s="139" t="s">
+      <c r="H2" s="137" t="s">
         <v>58</v>
       </c>
       <c r="I2" s="130"/>
@@ -4852,10 +4944,10 @@
       </c>
       <c r="K2" s="130"/>
     </row>
-    <row r="3" spans="2:11" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="136"/>
-      <c r="D3" s="137"/>
-      <c r="E3" s="133"/>
+    <row r="3" spans="2:28" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="135"/>
+      <c r="D3" s="136"/>
+      <c r="E3" s="132"/>
       <c r="F3" s="70" t="s">
         <v>54</v>
       </c>
@@ -4875,34 +4967,38 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C4" s="134" t="s">
+    <row r="4" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="C4" s="133" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="138"/>
+      <c r="D4" s="134"/>
       <c r="E4" s="78">
         <v>0.501</v>
       </c>
       <c r="F4" s="77">
         <v>0.40500000000000003</v>
       </c>
-      <c r="G4" s="65"/>
+      <c r="G4" s="65">
+        <v>0.94599999999999995</v>
+      </c>
       <c r="H4" s="77">
         <v>0.52300000000000002</v>
       </c>
-      <c r="I4" s="65"/>
+      <c r="I4" s="65">
+        <v>0.94299999999999995</v>
+      </c>
       <c r="J4" s="77">
         <v>0.53400000000000003</v>
       </c>
-      <c r="K4" s="65"/>
-    </row>
-    <row r="5" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K4" s="65">
+        <v>0.98399999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="90" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="D5" s="138"/>
       <c r="E5" s="74">
         <v>0.65400000000000003</v>
       </c>
@@ -4925,123 +5021,132 @@
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="90"/>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
+    <row r="6" spans="2:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="90" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="138"/>
       <c r="E6" s="74">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="G6" s="23">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="I6" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="K6" s="23">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="7" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="90" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="138"/>
+      <c r="E7" s="75">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="F7" s="45">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="G7" s="23">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="I7" s="13">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="K7" s="23">
+        <v>0.98899999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="C8" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="138"/>
+      <c r="E8" s="74">
         <v>0.94799999999999995</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F8" s="5">
         <v>0.36699999999999999</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G8" s="23">
         <v>0.96599999999999997</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H8" s="5">
         <v>0.69599999999999995</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I8" s="13">
         <v>0.97399999999999998</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J8" s="5">
         <v>0.79600000000000004</v>
       </c>
-      <c r="K6" s="23">
+      <c r="K8" s="23">
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="90" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="74">
-        <v>0.73499999999999999</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0.38600000000000001</v>
-      </c>
-      <c r="G7" s="23">
-        <v>0.95699999999999996</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0.60099999999999998</v>
-      </c>
-      <c r="I7" s="13">
-        <v>0.95</v>
-      </c>
-      <c r="J7" s="5">
-        <v>0.66200000000000003</v>
-      </c>
-      <c r="K7" s="23">
-        <v>0.995</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C8" s="90"/>
-      <c r="D8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="74">
+    <row r="9" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="90" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="138"/>
+      <c r="E9" s="74">
         <v>0.98699999999999999</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F9" s="5">
         <v>0.378</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G9" s="23">
         <v>0.95199999999999996</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H9" s="5">
         <v>0.70599999999999996</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I9" s="13">
         <v>0.98799999999999999</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J9" s="5">
         <v>0.84799999999999998</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K9" s="13">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="90" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="75">
-        <v>0.71499999999999997</v>
-      </c>
-      <c r="F9" s="45">
-        <v>0.39400000000000002</v>
-      </c>
-      <c r="G9" s="23">
-        <v>0.96099999999999997</v>
-      </c>
-      <c r="H9" s="5">
-        <v>0.58399999999999996</v>
-      </c>
-      <c r="I9" s="13">
-        <v>0.94399999999999995</v>
-      </c>
-      <c r="J9" s="5">
-        <v>0.66700000000000004</v>
-      </c>
-      <c r="K9" s="23">
-        <v>0.98899999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="131"/>
-      <c r="D10" s="43" t="s">
-        <v>19</v>
-      </c>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="10"/>
+      <c r="AA9" s="10"/>
+      <c r="AB9" s="10"/>
+    </row>
+    <row r="10" spans="2:28" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="139" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="140"/>
       <c r="E10" s="76">
         <v>0.99</v>
       </c>
@@ -5063,115 +5168,300 @@
       <c r="K10" s="66">
         <v>0.99399999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G12" s="5"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+      <c r="AA10" s="10"/>
+      <c r="AB10" s="10"/>
+    </row>
+    <row r="11" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="10"/>
+      <c r="AB11" s="10"/>
+    </row>
+    <row r="12" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="G12" s="5">
+        <f>(G4-$E4)/$E4</f>
+        <v>0.88822355289421151</v>
+      </c>
       <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="I12" s="5">
+        <f>(I4-$E4)/$E4</f>
+        <v>0.88223552894211565</v>
+      </c>
       <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G13" s="5"/>
+      <c r="K12" s="5">
+        <f>(K4-$E4)/$E4</f>
+        <v>0.96407185628742509</v>
+      </c>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="10"/>
+      <c r="AA12" s="10"/>
+      <c r="AB12" s="10"/>
+    </row>
+    <row r="13" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="G13" s="5">
+        <f>(G5-$E5)/$E5</f>
+        <v>0.44495412844036686</v>
+      </c>
       <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="I13" s="5">
+        <f>(I5-$E5)/$E5</f>
+        <v>0.46330275229357787</v>
+      </c>
       <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G14" s="5"/>
+      <c r="K13" s="5">
+        <f>(K5-$E5)/$E5</f>
+        <v>0.51681957186544336</v>
+      </c>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="10"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="10"/>
+      <c r="AA13" s="10"/>
+      <c r="AB13" s="10"/>
+    </row>
+    <row r="14" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="G14" s="5">
+        <f t="shared" ref="G14:I18" si="0">(G6-$E6)/$E6</f>
+        <v>0.30204081632653057</v>
+      </c>
       <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="I14" s="5">
+        <f t="shared" si="0"/>
+        <v>0.29251700680272102</v>
+      </c>
       <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G15" s="5"/>
+      <c r="K14" s="5">
+        <f t="shared" ref="K14" si="1">(K6-$E6)/$E6</f>
+        <v>0.35374149659863946</v>
+      </c>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="10"/>
+      <c r="AA14" s="10"/>
+      <c r="AB14" s="10"/>
+    </row>
+    <row r="15" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="G15" s="5">
+        <f t="shared" si="0"/>
+        <v>0.34405594405594409</v>
+      </c>
       <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="I15" s="5">
+        <f t="shared" si="0"/>
+        <v>0.32027972027972029</v>
+      </c>
       <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G16" s="5"/>
+      <c r="K15" s="5">
+        <f t="shared" ref="K15" si="2">(K7-$E7)/$E7</f>
+        <v>0.38321678321678326</v>
+      </c>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="10"/>
+      <c r="AA15" s="10"/>
+      <c r="AB15" s="10"/>
+    </row>
+    <row r="16" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="G16" s="5">
+        <f t="shared" si="0"/>
+        <v>1.8987341772151917E-2</v>
+      </c>
       <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
+      <c r="I16" s="5">
+        <f t="shared" si="0"/>
+        <v>2.7426160337552768E-2</v>
+      </c>
       <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
+      <c r="K16" s="5">
+        <f t="shared" ref="K16" si="3">(K8-$E8)/$E8</f>
+        <v>2.9535864978902981E-2</v>
+      </c>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="10"/>
+      <c r="AB16" s="10"/>
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C17" s="42"/>
       <c r="D17" s="42"/>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5">
+        <f t="shared" si="0"/>
+        <v>-3.5460992907801449E-2</v>
+      </c>
       <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
+      <c r="I17" s="5">
+        <f t="shared" si="0"/>
+        <v>1.0131712259371843E-3</v>
+      </c>
       <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
+      <c r="K17" s="5">
+        <f t="shared" ref="K17" si="4">(K9-$E9)/$E9</f>
+        <v>3.0395136778115527E-3</v>
+      </c>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C18" s="42"/>
       <c r="D18" s="42"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
+      <c r="G18" s="5">
+        <f t="shared" si="0"/>
+        <v>-3.5353535353535387E-2</v>
+      </c>
+      <c r="I18" s="5">
+        <f t="shared" si="0"/>
+        <v>-1.010101010101011E-3</v>
+      </c>
+      <c r="K18" s="5">
+        <f t="shared" ref="K18" si="5">(K10-$E10)/$E10</f>
+        <v>4.0404040404040439E-3</v>
+      </c>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C19" s="42"/>
       <c r="D19" s="42"/>
       <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
       <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
       <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
+      <c r="G20" s="5">
+        <f>AVERAGE(G13:G15)</f>
+        <v>0.36368362960761386</v>
+      </c>
+      <c r="I20" s="5">
+        <f>AVERAGE(I13:I15)</f>
+        <v>0.3586998264586731</v>
+      </c>
+      <c r="K20" s="5">
+        <f>AVERAGE(K13:K15)</f>
+        <v>0.41792595056028864</v>
+      </c>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C21" s="42"/>
       <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
+      <c r="G21" s="5">
+        <f>AVERAGE(G16:G18)</f>
+        <v>-1.7275728829728308E-2</v>
+      </c>
+      <c r="I21" s="5">
+        <f>AVERAGE(I16:I18)</f>
+        <v>9.1430768511296476E-3</v>
+      </c>
+      <c r="K21" s="5">
+        <f>AVERAGE(K16:K18)</f>
+        <v>1.2205260899039526E-2</v>
+      </c>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C22" s="42"/>
       <c r="D22" s="42"/>
       <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
       <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
       <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
     <mergeCell ref="J2:K2"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="C2:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
   </mergeCells>
-  <conditionalFormatting sqref="E4:K10">
+  <conditionalFormatting sqref="E4:K7 E10:K10">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color theme="6" tint="-0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8:K8">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color theme="6" tint="-0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9:K9">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
created lots of visualizations
</commit_message>
<xml_diff>
--- a/visualizations/join_results.xlsx
+++ b/visualizations/join_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/visualizations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4AD315-474E-C64B-81BF-F2379F030D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A424EBF-E30C-A841-B759-F790AB1B6BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="4880" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="7480" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="heuristics" sheetId="10" r:id="rId1"/>
@@ -745,6 +745,48 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -754,62 +796,80 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -817,72 +877,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -895,6 +895,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -921,15 +930,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1329,52 +1329,52 @@
       <c r="D3" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="84" t="s">
+      <c r="F3" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="86"/>
-      <c r="N3" s="84" t="s">
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="82"/>
+      <c r="N3" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
-      <c r="Q3" s="85"/>
-      <c r="R3" s="85"/>
-      <c r="S3" s="85"/>
-      <c r="T3" s="86"/>
-      <c r="U3" s="85" t="s">
+      <c r="O3" s="81"/>
+      <c r="P3" s="81"/>
+      <c r="Q3" s="81"/>
+      <c r="R3" s="81"/>
+      <c r="S3" s="81"/>
+      <c r="T3" s="82"/>
+      <c r="U3" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="V3" s="85"/>
-      <c r="W3" s="85"/>
-      <c r="X3" s="85"/>
-      <c r="Y3" s="86"/>
-      <c r="Z3" s="100" t="s">
+      <c r="V3" s="81"/>
+      <c r="W3" s="81"/>
+      <c r="X3" s="81"/>
+      <c r="Y3" s="82"/>
+      <c r="Z3" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="AA3" s="98"/>
-      <c r="AB3" s="98"/>
-      <c r="AC3" s="98"/>
-      <c r="AD3" s="99"/>
-      <c r="AE3" s="97" t="s">
+      <c r="AA3" s="90"/>
+      <c r="AB3" s="90"/>
+      <c r="AC3" s="90"/>
+      <c r="AD3" s="91"/>
+      <c r="AE3" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="AF3" s="98"/>
-      <c r="AG3" s="98"/>
-      <c r="AH3" s="98"/>
-      <c r="AI3" s="99"/>
-      <c r="AJ3" s="97" t="s">
+      <c r="AF3" s="90"/>
+      <c r="AG3" s="90"/>
+      <c r="AH3" s="90"/>
+      <c r="AI3" s="91"/>
+      <c r="AJ3" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="AK3" s="98"/>
-      <c r="AL3" s="98"/>
-      <c r="AM3" s="98"/>
-      <c r="AN3" s="99"/>
+      <c r="AK3" s="90"/>
+      <c r="AL3" s="90"/>
+      <c r="AM3" s="90"/>
+      <c r="AN3" s="91"/>
       <c r="AP3" s="18"/>
       <c r="AQ3" s="21" t="s">
         <v>18</v>
@@ -1390,7 +1390,7 @@
       </c>
     </row>
     <row r="4" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="95" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="21">
@@ -1399,52 +1399,52 @@
       <c r="D4" s="41">
         <v>0.86699999999999999</v>
       </c>
-      <c r="F4" s="89"/>
-      <c r="G4" s="87"/>
-      <c r="H4" s="87" t="s">
+      <c r="F4" s="86"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="87"/>
-      <c r="J4" s="87"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="88"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="87" t="s">
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="83"/>
+      <c r="L4" s="84"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="83"/>
+      <c r="P4" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="87"/>
-      <c r="R4" s="87"/>
-      <c r="S4" s="87"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="87" t="s">
+      <c r="Q4" s="83"/>
+      <c r="R4" s="83"/>
+      <c r="S4" s="83"/>
+      <c r="T4" s="84"/>
+      <c r="U4" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="V4" s="87"/>
-      <c r="W4" s="87"/>
-      <c r="X4" s="87"/>
-      <c r="Y4" s="88"/>
-      <c r="Z4" s="87" t="s">
+      <c r="V4" s="83"/>
+      <c r="W4" s="83"/>
+      <c r="X4" s="83"/>
+      <c r="Y4" s="84"/>
+      <c r="Z4" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="AA4" s="87"/>
-      <c r="AB4" s="87"/>
-      <c r="AC4" s="87"/>
-      <c r="AD4" s="88"/>
-      <c r="AE4" s="87" t="s">
+      <c r="AA4" s="83"/>
+      <c r="AB4" s="83"/>
+      <c r="AC4" s="83"/>
+      <c r="AD4" s="84"/>
+      <c r="AE4" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="AF4" s="87"/>
-      <c r="AG4" s="87"/>
-      <c r="AH4" s="87"/>
-      <c r="AI4" s="88"/>
-      <c r="AJ4" s="87" t="s">
+      <c r="AF4" s="83"/>
+      <c r="AG4" s="83"/>
+      <c r="AH4" s="83"/>
+      <c r="AI4" s="84"/>
+      <c r="AJ4" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="AK4" s="87"/>
-      <c r="AL4" s="87"/>
-      <c r="AM4" s="87"/>
-      <c r="AN4" s="88"/>
+      <c r="AK4" s="83"/>
+      <c r="AL4" s="83"/>
+      <c r="AM4" s="83"/>
+      <c r="AN4" s="84"/>
       <c r="AP4" s="29" t="s">
         <v>48</v>
       </c>
@@ -1466,15 +1466,15 @@
       </c>
     </row>
     <row r="5" spans="2:46" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="82"/>
+      <c r="B5" s="79"/>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="25">
         <v>0.90800000000000003</v>
       </c>
-      <c r="F5" s="90"/>
-      <c r="G5" s="91"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="88"/>
       <c r="H5" s="1">
         <v>1</v>
       </c>
@@ -1491,8 +1491,8 @@
         <v>5</v>
       </c>
       <c r="M5" s="24"/>
-      <c r="N5" s="90"/>
-      <c r="O5" s="91"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="88"/>
       <c r="P5" s="1">
         <v>1</v>
       </c>
@@ -1589,14 +1589,14 @@
       </c>
     </row>
     <row r="6" spans="2:46" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="82"/>
+      <c r="B6" s="79"/>
       <c r="C6" s="1">
         <v>5</v>
       </c>
       <c r="D6" s="25">
         <v>0.94599999999999995</v>
       </c>
-      <c r="F6" s="82" t="s">
+      <c r="F6" s="79" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="1">
@@ -1618,7 +1618,7 @@
         <v>0.83740632127728898</v>
       </c>
       <c r="M6" s="24"/>
-      <c r="N6" s="82" t="s">
+      <c r="N6" s="79" t="s">
         <v>4</v>
       </c>
       <c r="O6" s="1">
@@ -1720,14 +1720,14 @@
       </c>
     </row>
     <row r="7" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="82"/>
+      <c r="B7" s="79"/>
       <c r="C7" s="1">
         <v>10</v>
       </c>
       <c r="D7" s="25">
         <v>0.94799999999999995</v>
       </c>
-      <c r="F7" s="82"/>
+      <c r="F7" s="79"/>
       <c r="G7" s="1">
         <v>2</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>0.88302400000000003</v>
       </c>
       <c r="M7" s="24"/>
-      <c r="N7" s="82"/>
+      <c r="N7" s="79"/>
       <c r="O7" s="1">
         <v>2</v>
       </c>
@@ -1828,14 +1828,14 @@
       </c>
     </row>
     <row r="8" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="83"/>
+      <c r="B8" s="80"/>
       <c r="C8" s="15">
         <v>20</v>
       </c>
       <c r="D8" s="27">
         <v>0.93400000000000005</v>
       </c>
-      <c r="F8" s="82"/>
+      <c r="F8" s="79"/>
       <c r="G8" s="1">
         <v>5</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>0.91756300000000002</v>
       </c>
       <c r="M8" s="24"/>
-      <c r="N8" s="82"/>
+      <c r="N8" s="79"/>
       <c r="O8" s="1">
         <v>5</v>
       </c>
@@ -1940,7 +1940,7 @@
       </c>
     </row>
     <row r="9" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B9" s="81" t="s">
+      <c r="B9" s="95" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="21">
@@ -1949,7 +1949,7 @@
       <c r="D9" s="41">
         <v>0.83799999999999997</v>
       </c>
-      <c r="F9" s="82"/>
+      <c r="F9" s="79"/>
       <c r="G9" s="1">
         <v>10</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>0.92538299999999996</v>
       </c>
       <c r="M9" s="24"/>
-      <c r="N9" s="82"/>
+      <c r="N9" s="79"/>
       <c r="O9" s="1">
         <v>10</v>
       </c>
@@ -2054,14 +2054,14 @@
       </c>
     </row>
     <row r="10" spans="2:46" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="82"/>
+      <c r="B10" s="79"/>
       <c r="C10" s="1">
         <v>2</v>
       </c>
       <c r="D10" s="25">
         <v>0.84699999999999998</v>
       </c>
-      <c r="F10" s="83"/>
+      <c r="F10" s="80"/>
       <c r="G10" s="15">
         <v>20</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>0.92049499999999995</v>
       </c>
       <c r="M10" s="24"/>
-      <c r="N10" s="83"/>
+      <c r="N10" s="80"/>
       <c r="O10" s="15">
         <v>20</v>
       </c>
@@ -2166,22 +2166,22 @@
       </c>
     </row>
     <row r="11" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="82"/>
+      <c r="B11" s="79"/>
       <c r="C11" s="1">
         <v>3</v>
       </c>
       <c r="D11" s="25">
         <v>0.85099999999999998</v>
       </c>
-      <c r="F11" s="89"/>
-      <c r="G11" s="87"/>
-      <c r="H11" s="87" t="s">
+      <c r="F11" s="86"/>
+      <c r="G11" s="83"/>
+      <c r="H11" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="87"/>
-      <c r="J11" s="87"/>
-      <c r="K11" s="87"/>
-      <c r="L11" s="88"/>
+      <c r="I11" s="83"/>
+      <c r="J11" s="83"/>
+      <c r="K11" s="83"/>
+      <c r="L11" s="84"/>
       <c r="M11" s="24"/>
       <c r="N11" s="42"/>
       <c r="P11" s="24"/>
@@ -2191,15 +2191,15 @@
       <c r="T11" s="24"/>
     </row>
     <row r="12" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="82"/>
+      <c r="B12" s="79"/>
       <c r="C12" s="1">
         <v>4</v>
       </c>
       <c r="D12" s="25">
         <v>0.85199999999999998</v>
       </c>
-      <c r="F12" s="90"/>
-      <c r="G12" s="91"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="88"/>
       <c r="H12" s="1">
         <v>0.1</v>
       </c>
@@ -2224,14 +2224,14 @@
       </c>
     </row>
     <row r="13" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="83"/>
+      <c r="B13" s="80"/>
       <c r="C13" s="15">
         <v>5</v>
       </c>
       <c r="D13" s="27">
         <v>0.83499999999999996</v>
       </c>
-      <c r="F13" s="82" t="s">
+      <c r="F13" s="79" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="1">
@@ -2254,7 +2254,7 @@
       </c>
     </row>
     <row r="14" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="81" t="s">
+      <c r="B14" s="95" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="21">
@@ -2263,7 +2263,7 @@
       <c r="D14" s="41">
         <v>0.65500000000000003</v>
       </c>
-      <c r="F14" s="82"/>
+      <c r="F14" s="79"/>
       <c r="G14" s="1">
         <v>2</v>
       </c>
@@ -2287,14 +2287,14 @@
       <c r="O14" s="24"/>
     </row>
     <row r="15" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B15" s="82"/>
+      <c r="B15" s="79"/>
       <c r="C15" s="1">
         <v>0.2</v>
       </c>
       <c r="D15" s="25">
         <v>0.70099999999999996</v>
       </c>
-      <c r="F15" s="82"/>
+      <c r="F15" s="79"/>
       <c r="G15" s="1">
         <v>5</v>
       </c>
@@ -2317,14 +2317,14 @@
       <c r="P15" s="5"/>
     </row>
     <row r="16" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B16" s="82"/>
+      <c r="B16" s="79"/>
       <c r="C16" s="1">
         <v>0.3</v>
       </c>
       <c r="D16" s="25">
         <v>0.73499999999999999</v>
       </c>
-      <c r="F16" s="82"/>
+      <c r="F16" s="79"/>
       <c r="G16" s="1">
         <v>10</v>
       </c>
@@ -2346,14 +2346,14 @@
       <c r="M16" s="24"/>
     </row>
     <row r="17" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="82"/>
+      <c r="B17" s="79"/>
       <c r="C17" s="1">
         <v>0.4</v>
       </c>
       <c r="D17" s="25">
         <v>0.753</v>
       </c>
-      <c r="F17" s="83"/>
+      <c r="F17" s="80"/>
       <c r="G17" s="15">
         <v>20</v>
       </c>
@@ -2380,22 +2380,22 @@
       <c r="T17" s="24"/>
     </row>
     <row r="18" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="83"/>
+      <c r="B18" s="80"/>
       <c r="C18" s="15">
         <v>0.5</v>
       </c>
       <c r="D18" s="27">
         <v>0.65400000000000003</v>
       </c>
-      <c r="F18" s="92"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="93" t="s">
+      <c r="F18" s="96"/>
+      <c r="G18" s="97"/>
+      <c r="H18" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="93"/>
-      <c r="J18" s="93"/>
-      <c r="K18" s="93"/>
-      <c r="L18" s="96"/>
+      <c r="I18" s="97"/>
+      <c r="J18" s="97"/>
+      <c r="K18" s="97"/>
+      <c r="L18" s="100"/>
       <c r="N18" s="42"/>
       <c r="P18" s="24"/>
       <c r="Q18" s="24"/>
@@ -2404,8 +2404,8 @@
       <c r="T18" s="24"/>
     </row>
     <row r="19" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F19" s="94"/>
-      <c r="G19" s="95"/>
+      <c r="F19" s="98"/>
+      <c r="G19" s="99"/>
       <c r="H19" s="1">
         <v>0.1</v>
       </c>
@@ -2429,7 +2429,7 @@
       <c r="T19" s="24"/>
     </row>
     <row r="20" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="79" t="s">
+      <c r="F20" s="93" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="44">
@@ -2453,7 +2453,7 @@
       <c r="P20" s="24"/>
     </row>
     <row r="21" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="79"/>
+      <c r="F21" s="93"/>
       <c r="G21" s="44">
         <v>2</v>
       </c>
@@ -2474,7 +2474,7 @@
       </c>
     </row>
     <row r="22" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F22" s="79"/>
+      <c r="F22" s="93"/>
       <c r="G22" s="44">
         <v>3</v>
       </c>
@@ -2496,7 +2496,7 @@
     </row>
     <row r="23" spans="2:40" x14ac:dyDescent="0.2">
       <c r="D23" s="42"/>
-      <c r="F23" s="79"/>
+      <c r="F23" s="93"/>
       <c r="G23" s="44">
         <v>4</v>
       </c>
@@ -2520,7 +2520,7 @@
     </row>
     <row r="24" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D24" s="42"/>
-      <c r="F24" s="80"/>
+      <c r="F24" s="94"/>
       <c r="G24" s="43">
         <v>5</v>
       </c>
@@ -3026,18 +3026,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="N6:N10"/>
-    <mergeCell ref="U3:Y3"/>
-    <mergeCell ref="U4:Y4"/>
-    <mergeCell ref="N3:T3"/>
-    <mergeCell ref="N4:O5"/>
-    <mergeCell ref="P4:T4"/>
-    <mergeCell ref="AJ3:AN3"/>
-    <mergeCell ref="AJ4:AN4"/>
-    <mergeCell ref="Z3:AD3"/>
-    <mergeCell ref="Z4:AD4"/>
-    <mergeCell ref="AE3:AI3"/>
-    <mergeCell ref="AE4:AI4"/>
     <mergeCell ref="F20:F24"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B14:B18"/>
@@ -3051,6 +3039,18 @@
     <mergeCell ref="F13:F17"/>
     <mergeCell ref="F18:G19"/>
     <mergeCell ref="H18:L18"/>
+    <mergeCell ref="AJ3:AN3"/>
+    <mergeCell ref="AJ4:AN4"/>
+    <mergeCell ref="Z3:AD3"/>
+    <mergeCell ref="Z4:AD4"/>
+    <mergeCell ref="AE3:AI3"/>
+    <mergeCell ref="AE4:AI4"/>
+    <mergeCell ref="N6:N10"/>
+    <mergeCell ref="U3:Y3"/>
+    <mergeCell ref="U4:Y4"/>
+    <mergeCell ref="N3:T3"/>
+    <mergeCell ref="N4:O5"/>
+    <mergeCell ref="P4:T4"/>
   </mergeCells>
   <conditionalFormatting sqref="D31:D43 R33:AD33 H33:L35 P33:P35 AJ33:AN35 R34:AC35 H38:L38 H39:H42 K39:L42 H45:L49">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -3106,7 +3106,7 @@
   <dimension ref="B1:W29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J29" activeCellId="1" sqref="J22:K22 J29:K29"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3127,26 +3127,26 @@
     <row r="1" spans="2:20" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B2" s="53"/>
-      <c r="D2" s="113" t="s">
+      <c r="D2" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="114" t="s">
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="114"/>
-      <c r="J2" s="114"/>
-      <c r="K2" s="114"/>
-      <c r="L2" s="115"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="103"/>
     </row>
     <row r="3" spans="2:20" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="53"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="118"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="106"/>
       <c r="H3" s="59" t="s">
         <v>53</v>
       </c>
@@ -3167,178 +3167,178 @@
       <c r="B4" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="119" t="s">
+      <c r="D4" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="120"/>
-      <c r="F4" s="122" t="s">
+      <c r="E4" s="108"/>
+      <c r="F4" s="112" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="109">
+      <c r="H4" s="114">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="109"/>
-      <c r="J4" s="109"/>
-      <c r="K4" s="109"/>
-      <c r="L4" s="110"/>
+      <c r="I4" s="114"/>
+      <c r="J4" s="114"/>
+      <c r="K4" s="114"/>
+      <c r="L4" s="115"/>
     </row>
     <row r="5" spans="2:20" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="103"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="112"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="113"/>
       <c r="G5" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="123">
+      <c r="H5" s="116">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="123"/>
-      <c r="J5" s="123"/>
-      <c r="K5" s="123"/>
-      <c r="L5" s="124"/>
+      <c r="I5" s="116"/>
+      <c r="J5" s="116"/>
+      <c r="K5" s="116"/>
+      <c r="L5" s="117"/>
     </row>
     <row r="6" spans="2:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="103"/>
-      <c r="E6" s="120"/>
-      <c r="F6" s="122" t="s">
+      <c r="D6" s="109"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="112" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="107">
+      <c r="H6" s="118">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="107"/>
-      <c r="J6" s="107"/>
-      <c r="K6" s="107"/>
-      <c r="L6" s="108"/>
+      <c r="I6" s="118"/>
+      <c r="J6" s="118"/>
+      <c r="K6" s="118"/>
+      <c r="L6" s="119"/>
     </row>
     <row r="7" spans="2:20" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="52"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="120"/>
-      <c r="F7" s="112"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="113"/>
       <c r="G7" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="123">
+      <c r="H7" s="116">
         <v>0.85199999999999998</v>
       </c>
-      <c r="I7" s="123"/>
-      <c r="J7" s="123"/>
-      <c r="K7" s="123"/>
-      <c r="L7" s="124"/>
+      <c r="I7" s="116"/>
+      <c r="J7" s="116"/>
+      <c r="K7" s="116"/>
+      <c r="L7" s="117"/>
     </row>
     <row r="8" spans="2:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="53"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="120"/>
-      <c r="F8" s="122" t="s">
+      <c r="D8" s="109"/>
+      <c r="E8" s="108"/>
+      <c r="F8" s="112" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="107">
+      <c r="H8" s="118">
         <v>0.65400000000000003</v>
       </c>
-      <c r="I8" s="107"/>
-      <c r="J8" s="107"/>
-      <c r="K8" s="107"/>
-      <c r="L8" s="108"/>
+      <c r="I8" s="118"/>
+      <c r="J8" s="118"/>
+      <c r="K8" s="118"/>
+      <c r="L8" s="119"/>
     </row>
     <row r="9" spans="2:20" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="53"/>
-      <c r="D9" s="103"/>
-      <c r="E9" s="120"/>
-      <c r="F9" s="112"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="108"/>
+      <c r="F9" s="113"/>
       <c r="G9" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="123">
+      <c r="H9" s="116">
         <v>0.753</v>
       </c>
-      <c r="I9" s="123"/>
-      <c r="J9" s="123"/>
-      <c r="K9" s="123"/>
-      <c r="L9" s="124"/>
+      <c r="I9" s="116"/>
+      <c r="J9" s="116"/>
+      <c r="K9" s="116"/>
+      <c r="L9" s="117"/>
     </row>
     <row r="10" spans="2:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="103"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="122" t="s">
+      <c r="D10" s="109"/>
+      <c r="E10" s="108"/>
+      <c r="F10" s="112" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="107">
+      <c r="H10" s="118">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I10" s="107"/>
-      <c r="J10" s="107"/>
-      <c r="K10" s="107"/>
-      <c r="L10" s="108"/>
+      <c r="I10" s="118"/>
+      <c r="J10" s="118"/>
+      <c r="K10" s="118"/>
+      <c r="L10" s="119"/>
     </row>
     <row r="11" spans="2:20" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="103"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="112"/>
+      <c r="D11" s="109"/>
+      <c r="E11" s="108"/>
+      <c r="F11" s="113"/>
       <c r="G11" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="123">
+      <c r="H11" s="116">
         <v>0.98699999999999999</v>
       </c>
-      <c r="I11" s="123"/>
-      <c r="J11" s="123"/>
-      <c r="K11" s="123"/>
-      <c r="L11" s="124"/>
+      <c r="I11" s="116"/>
+      <c r="J11" s="116"/>
+      <c r="K11" s="116"/>
+      <c r="L11" s="117"/>
     </row>
     <row r="12" spans="2:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="103"/>
-      <c r="E12" s="120"/>
-      <c r="F12" s="122" t="s">
+      <c r="D12" s="109"/>
+      <c r="E12" s="108"/>
+      <c r="F12" s="112" t="s">
         <v>21</v>
       </c>
       <c r="G12" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="107">
+      <c r="H12" s="118">
         <v>0.71499999999999997</v>
       </c>
-      <c r="I12" s="107"/>
-      <c r="J12" s="107"/>
-      <c r="K12" s="107"/>
-      <c r="L12" s="108"/>
+      <c r="I12" s="118"/>
+      <c r="J12" s="118"/>
+      <c r="K12" s="118"/>
+      <c r="L12" s="119"/>
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
     <row r="13" spans="2:20" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="105"/>
-      <c r="E13" s="121"/>
-      <c r="F13" s="111"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="120"/>
       <c r="G13" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="109">
+      <c r="H13" s="114">
         <v>0.99</v>
       </c>
-      <c r="I13" s="109"/>
-      <c r="J13" s="109"/>
-      <c r="K13" s="109"/>
-      <c r="L13" s="110"/>
+      <c r="I13" s="114"/>
+      <c r="J13" s="114"/>
+      <c r="K13" s="114"/>
+      <c r="L13" s="115"/>
       <c r="P13" s="72"/>
       <c r="Q13" s="72"/>
       <c r="R13" s="72"/>
@@ -3346,14 +3346,14 @@
       <c r="T13" s="72"/>
     </row>
     <row r="14" spans="2:20" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="101" t="s">
+      <c r="D14" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="102"/>
-      <c r="F14" s="84" t="s">
+      <c r="E14" s="122"/>
+      <c r="F14" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="86"/>
+      <c r="G14" s="82"/>
       <c r="H14" s="67">
         <v>0.52</v>
       </c>
@@ -3392,9 +3392,9 @@
       </c>
     </row>
     <row r="15" spans="2:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="103"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="111" t="s">
+      <c r="D15" s="109"/>
+      <c r="E15" s="123"/>
+      <c r="F15" s="120" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -3438,9 +3438,9 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D16" s="103"/>
-      <c r="E16" s="104"/>
-      <c r="F16" s="111"/>
+      <c r="D16" s="109"/>
+      <c r="E16" s="123"/>
+      <c r="F16" s="120"/>
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
@@ -3466,9 +3466,9 @@
       <c r="S16" s="31"/>
     </row>
     <row r="17" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D17" s="103"/>
-      <c r="E17" s="104"/>
-      <c r="F17" s="111"/>
+      <c r="D17" s="109"/>
+      <c r="E17" s="123"/>
+      <c r="F17" s="120"/>
       <c r="G17" s="1" t="s">
         <v>22</v>
       </c>
@@ -3495,9 +3495,9 @@
       <c r="W17" s="5"/>
     </row>
     <row r="18" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D18" s="103"/>
-      <c r="E18" s="104"/>
-      <c r="F18" s="111"/>
+      <c r="D18" s="109"/>
+      <c r="E18" s="123"/>
+      <c r="F18" s="120"/>
       <c r="G18" s="1" t="s">
         <v>45</v>
       </c>
@@ -3523,9 +3523,9 @@
       <c r="S18" s="31"/>
     </row>
     <row r="19" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D19" s="103"/>
-      <c r="E19" s="104"/>
-      <c r="F19" s="111"/>
+      <c r="D19" s="109"/>
+      <c r="E19" s="123"/>
+      <c r="F19" s="120"/>
       <c r="G19" s="1" t="s">
         <v>46</v>
       </c>
@@ -3551,9 +3551,9 @@
       <c r="S19" s="31"/>
     </row>
     <row r="20" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D20" s="103"/>
-      <c r="E20" s="104"/>
-      <c r="F20" s="111"/>
+      <c r="D20" s="109"/>
+      <c r="E20" s="123"/>
+      <c r="F20" s="120"/>
       <c r="G20" s="1" t="s">
         <v>47</v>
       </c>
@@ -3579,9 +3579,9 @@
       <c r="S20" s="31"/>
     </row>
     <row r="21" spans="4:23" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="103"/>
-      <c r="E21" s="104"/>
-      <c r="F21" s="112"/>
+      <c r="D21" s="109"/>
+      <c r="E21" s="123"/>
+      <c r="F21" s="113"/>
       <c r="G21" s="15" t="s">
         <v>21</v>
       </c>
@@ -3607,14 +3607,14 @@
       <c r="S21" s="31"/>
     </row>
     <row r="22" spans="4:23" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="103" t="s">
+      <c r="D22" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="104"/>
-      <c r="F22" s="84" t="s">
+      <c r="E22" s="123"/>
+      <c r="F22" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="86"/>
+      <c r="G22" s="82"/>
       <c r="H22" s="68">
         <v>0.495</v>
       </c>
@@ -3637,9 +3637,9 @@
       <c r="S22" s="31"/>
     </row>
     <row r="23" spans="4:23" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="103"/>
-      <c r="E23" s="104"/>
-      <c r="F23" s="111" t="s">
+      <c r="D23" s="109"/>
+      <c r="E23" s="123"/>
+      <c r="F23" s="120" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -3673,9 +3673,9 @@
       </c>
     </row>
     <row r="24" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D24" s="103"/>
-      <c r="E24" s="104"/>
-      <c r="F24" s="111"/>
+      <c r="D24" s="109"/>
+      <c r="E24" s="123"/>
+      <c r="F24" s="120"/>
       <c r="G24" s="1" t="s">
         <v>12</v>
       </c>
@@ -3707,9 +3707,9 @@
       </c>
     </row>
     <row r="25" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D25" s="103"/>
-      <c r="E25" s="104"/>
-      <c r="F25" s="111"/>
+      <c r="D25" s="109"/>
+      <c r="E25" s="123"/>
+      <c r="F25" s="120"/>
       <c r="G25" s="1" t="s">
         <v>22</v>
       </c>
@@ -3735,9 +3735,9 @@
       <c r="S25" s="31"/>
     </row>
     <row r="26" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D26" s="103"/>
-      <c r="E26" s="104"/>
-      <c r="F26" s="111"/>
+      <c r="D26" s="109"/>
+      <c r="E26" s="123"/>
+      <c r="F26" s="120"/>
       <c r="G26" s="1" t="s">
         <v>45</v>
       </c>
@@ -3763,9 +3763,9 @@
       <c r="S26" s="31"/>
     </row>
     <row r="27" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D27" s="103"/>
-      <c r="E27" s="104"/>
-      <c r="F27" s="111"/>
+      <c r="D27" s="109"/>
+      <c r="E27" s="123"/>
+      <c r="F27" s="120"/>
       <c r="G27" s="1" t="s">
         <v>46</v>
       </c>
@@ -3791,9 +3791,9 @@
       <c r="S27" s="31"/>
     </row>
     <row r="28" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D28" s="103"/>
-      <c r="E28" s="104"/>
-      <c r="F28" s="111"/>
+      <c r="D28" s="109"/>
+      <c r="E28" s="123"/>
+      <c r="F28" s="120"/>
       <c r="G28" s="1" t="s">
         <v>47</v>
       </c>
@@ -3819,9 +3819,9 @@
       <c r="S28" s="31"/>
     </row>
     <row r="29" spans="4:23" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="105"/>
-      <c r="E29" s="106"/>
-      <c r="F29" s="112"/>
+      <c r="D29" s="110"/>
+      <c r="E29" s="124"/>
+      <c r="F29" s="113"/>
       <c r="G29" s="15" t="s">
         <v>21</v>
       </c>
@@ -3848,6 +3848,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="D14:E21"/>
+    <mergeCell ref="D22:E29"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="F15:F21"/>
+    <mergeCell ref="F23:F29"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F22:G22"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D4:E13"/>
@@ -3864,14 +3872,6 @@
     <mergeCell ref="H10:L10"/>
     <mergeCell ref="H11:L11"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="D14:E21"/>
-    <mergeCell ref="D22:E29"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="F15:F21"/>
-    <mergeCell ref="F23:F29"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F22:G22"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:L29">
     <cfRule type="colorScale" priority="52">
@@ -3894,8 +3894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B202F2B-277F-994F-8FBA-31A55EB8F243}">
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J27" sqref="J27:K27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3916,26 +3916,26 @@
     <row r="1" spans="2:21" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B2" s="53"/>
-      <c r="D2" s="113" t="s">
+      <c r="D2" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="114" t="s">
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="114"/>
-      <c r="J2" s="114"/>
-      <c r="K2" s="114"/>
-      <c r="L2" s="115"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="103"/>
     </row>
     <row r="3" spans="2:21" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="53"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="118"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="106"/>
       <c r="H3" s="59" t="s">
         <v>53</v>
       </c>
@@ -3956,11 +3956,11 @@
       <c r="B4" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="119" t="s">
+      <c r="D4" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="120"/>
-      <c r="F4" s="122" t="s">
+      <c r="E4" s="108"/>
+      <c r="F4" s="112" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="63" t="s">
@@ -3969,169 +3969,169 @@
       <c r="H4" s="125">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="107"/>
-      <c r="J4" s="107"/>
-      <c r="K4" s="107"/>
-      <c r="L4" s="108"/>
+      <c r="I4" s="118"/>
+      <c r="J4" s="118"/>
+      <c r="K4" s="118"/>
+      <c r="L4" s="119"/>
     </row>
     <row r="5" spans="2:21" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="103"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="112"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="113"/>
       <c r="G5" s="64" t="s">
         <v>36</v>
       </c>
       <c r="H5" s="126">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="123"/>
-      <c r="J5" s="123"/>
-      <c r="K5" s="123"/>
-      <c r="L5" s="124"/>
+      <c r="I5" s="116"/>
+      <c r="J5" s="116"/>
+      <c r="K5" s="116"/>
+      <c r="L5" s="117"/>
     </row>
     <row r="6" spans="2:21" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="103"/>
-      <c r="E6" s="120"/>
-      <c r="F6" s="122" t="s">
+      <c r="D6" s="109"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="112" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="107">
+      <c r="H6" s="118">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="107"/>
-      <c r="J6" s="107"/>
-      <c r="K6" s="107"/>
-      <c r="L6" s="108"/>
+      <c r="I6" s="118"/>
+      <c r="J6" s="118"/>
+      <c r="K6" s="118"/>
+      <c r="L6" s="119"/>
     </row>
     <row r="7" spans="2:21" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="52"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="120"/>
-      <c r="F7" s="112"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="113"/>
       <c r="G7" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="123">
+      <c r="H7" s="116">
         <v>0.85199999999999998</v>
       </c>
-      <c r="I7" s="123"/>
-      <c r="J7" s="123"/>
-      <c r="K7" s="123"/>
-      <c r="L7" s="124"/>
+      <c r="I7" s="116"/>
+      <c r="J7" s="116"/>
+      <c r="K7" s="116"/>
+      <c r="L7" s="117"/>
     </row>
     <row r="8" spans="2:21" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="53"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="120"/>
-      <c r="F8" s="122" t="s">
+      <c r="D8" s="109"/>
+      <c r="E8" s="108"/>
+      <c r="F8" s="112" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="107">
+      <c r="H8" s="118">
         <v>0.65400000000000003</v>
       </c>
-      <c r="I8" s="107"/>
-      <c r="J8" s="107"/>
-      <c r="K8" s="107"/>
-      <c r="L8" s="108"/>
+      <c r="I8" s="118"/>
+      <c r="J8" s="118"/>
+      <c r="K8" s="118"/>
+      <c r="L8" s="119"/>
     </row>
     <row r="9" spans="2:21" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="53"/>
-      <c r="D9" s="103"/>
-      <c r="E9" s="120"/>
-      <c r="F9" s="112"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="108"/>
+      <c r="F9" s="113"/>
       <c r="G9" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="123">
+      <c r="H9" s="116">
         <v>0.753</v>
       </c>
-      <c r="I9" s="123"/>
-      <c r="J9" s="123"/>
-      <c r="K9" s="123"/>
-      <c r="L9" s="124"/>
+      <c r="I9" s="116"/>
+      <c r="J9" s="116"/>
+      <c r="K9" s="116"/>
+      <c r="L9" s="117"/>
     </row>
     <row r="10" spans="2:21" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="103"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="122" t="s">
+      <c r="D10" s="109"/>
+      <c r="E10" s="108"/>
+      <c r="F10" s="112" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="107">
+      <c r="H10" s="118">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I10" s="107"/>
-      <c r="J10" s="107"/>
-      <c r="K10" s="107"/>
-      <c r="L10" s="108"/>
+      <c r="I10" s="118"/>
+      <c r="J10" s="118"/>
+      <c r="K10" s="118"/>
+      <c r="L10" s="119"/>
     </row>
     <row r="11" spans="2:21" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="103"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="112"/>
+      <c r="D11" s="109"/>
+      <c r="E11" s="108"/>
+      <c r="F11" s="113"/>
       <c r="G11" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="123">
+      <c r="H11" s="116">
         <v>0.98699999999999999</v>
       </c>
-      <c r="I11" s="123"/>
-      <c r="J11" s="123"/>
-      <c r="K11" s="123"/>
-      <c r="L11" s="124"/>
+      <c r="I11" s="116"/>
+      <c r="J11" s="116"/>
+      <c r="K11" s="116"/>
+      <c r="L11" s="117"/>
     </row>
     <row r="12" spans="2:21" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="103"/>
-      <c r="E12" s="120"/>
-      <c r="F12" s="122" t="s">
+      <c r="D12" s="109"/>
+      <c r="E12" s="108"/>
+      <c r="F12" s="112" t="s">
         <v>21</v>
       </c>
       <c r="G12" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="107">
+      <c r="H12" s="118">
         <v>0.71499999999999997</v>
       </c>
-      <c r="I12" s="107"/>
-      <c r="J12" s="107"/>
-      <c r="K12" s="107"/>
-      <c r="L12" s="108"/>
+      <c r="I12" s="118"/>
+      <c r="J12" s="118"/>
+      <c r="K12" s="118"/>
+      <c r="L12" s="119"/>
     </row>
     <row r="13" spans="2:21" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="105"/>
-      <c r="E13" s="121"/>
-      <c r="F13" s="111"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="120"/>
       <c r="G13" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="109">
+      <c r="H13" s="114">
         <v>0.99</v>
       </c>
-      <c r="I13" s="109"/>
-      <c r="J13" s="109"/>
-      <c r="K13" s="109"/>
-      <c r="L13" s="110"/>
+      <c r="I13" s="114"/>
+      <c r="J13" s="114"/>
+      <c r="K13" s="114"/>
+      <c r="L13" s="115"/>
     </row>
     <row r="14" spans="2:21" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="101" t="s">
+      <c r="D14" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="102"/>
-      <c r="F14" s="122" t="s">
+      <c r="E14" s="122"/>
+      <c r="F14" s="112" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="21" t="s">
@@ -4175,9 +4175,9 @@
       <c r="U14" s="5"/>
     </row>
     <row r="15" spans="2:21" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="103"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="111"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="123"/>
+      <c r="F15" s="120"/>
       <c r="G15" s="1" t="s">
         <v>12</v>
       </c>
@@ -4219,9 +4219,9 @@
       <c r="U15" s="5"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="D16" s="103"/>
-      <c r="E16" s="104"/>
-      <c r="F16" s="111"/>
+      <c r="D16" s="109"/>
+      <c r="E16" s="123"/>
+      <c r="F16" s="120"/>
       <c r="G16" s="1" t="s">
         <v>22</v>
       </c>
@@ -4242,9 +4242,9 @@
       </c>
     </row>
     <row r="17" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D17" s="103"/>
-      <c r="E17" s="104"/>
-      <c r="F17" s="111"/>
+      <c r="D17" s="109"/>
+      <c r="E17" s="123"/>
+      <c r="F17" s="120"/>
       <c r="G17" s="1" t="s">
         <v>45</v>
       </c>
@@ -4270,9 +4270,9 @@
       <c r="U17" s="5"/>
     </row>
     <row r="18" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D18" s="103"/>
-      <c r="E18" s="104"/>
-      <c r="F18" s="111"/>
+      <c r="D18" s="109"/>
+      <c r="E18" s="123"/>
+      <c r="F18" s="120"/>
       <c r="G18" s="1" t="s">
         <v>46</v>
       </c>
@@ -4293,9 +4293,9 @@
       </c>
     </row>
     <row r="19" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D19" s="103"/>
-      <c r="E19" s="104"/>
-      <c r="F19" s="111"/>
+      <c r="D19" s="109"/>
+      <c r="E19" s="123"/>
+      <c r="F19" s="120"/>
       <c r="G19" s="1" t="s">
         <v>47</v>
       </c>
@@ -4319,9 +4319,9 @@
       <c r="Q19" s="5"/>
     </row>
     <row r="20" spans="4:21" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="103"/>
-      <c r="E20" s="104"/>
-      <c r="F20" s="112"/>
+      <c r="D20" s="109"/>
+      <c r="E20" s="123"/>
+      <c r="F20" s="113"/>
       <c r="G20" s="15" t="s">
         <v>21</v>
       </c>
@@ -4342,11 +4342,11 @@
       </c>
     </row>
     <row r="21" spans="4:21" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="103" t="s">
+      <c r="D21" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="104"/>
-      <c r="F21" s="122" t="s">
+      <c r="E21" s="123"/>
+      <c r="F21" s="112" t="s">
         <v>10</v>
       </c>
       <c r="G21" s="1" t="s">
@@ -4369,9 +4369,9 @@
       </c>
     </row>
     <row r="22" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D22" s="103"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="111"/>
+      <c r="D22" s="109"/>
+      <c r="E22" s="123"/>
+      <c r="F22" s="120"/>
       <c r="G22" s="1" t="s">
         <v>12</v>
       </c>
@@ -4392,9 +4392,9 @@
       </c>
     </row>
     <row r="23" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D23" s="103"/>
-      <c r="E23" s="104"/>
-      <c r="F23" s="111"/>
+      <c r="D23" s="109"/>
+      <c r="E23" s="123"/>
+      <c r="F23" s="120"/>
       <c r="G23" s="1" t="s">
         <v>22</v>
       </c>
@@ -4415,9 +4415,9 @@
       </c>
     </row>
     <row r="24" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D24" s="103"/>
-      <c r="E24" s="104"/>
-      <c r="F24" s="111"/>
+      <c r="D24" s="109"/>
+      <c r="E24" s="123"/>
+      <c r="F24" s="120"/>
       <c r="G24" s="1" t="s">
         <v>45</v>
       </c>
@@ -4438,9 +4438,9 @@
       </c>
     </row>
     <row r="25" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D25" s="103"/>
-      <c r="E25" s="104"/>
-      <c r="F25" s="111"/>
+      <c r="D25" s="109"/>
+      <c r="E25" s="123"/>
+      <c r="F25" s="120"/>
       <c r="G25" s="1" t="s">
         <v>46</v>
       </c>
@@ -4461,9 +4461,9 @@
       </c>
     </row>
     <row r="26" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D26" s="103"/>
-      <c r="E26" s="104"/>
-      <c r="F26" s="111"/>
+      <c r="D26" s="109"/>
+      <c r="E26" s="123"/>
+      <c r="F26" s="120"/>
       <c r="G26" s="1" t="s">
         <v>47</v>
       </c>
@@ -4484,9 +4484,9 @@
       </c>
     </row>
     <row r="27" spans="4:21" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="105"/>
-      <c r="E27" s="106"/>
-      <c r="F27" s="112"/>
+      <c r="D27" s="110"/>
+      <c r="E27" s="124"/>
+      <c r="F27" s="113"/>
       <c r="G27" s="15" t="s">
         <v>21</v>
       </c>
@@ -4508,12 +4508,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="H10:L10"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="F14:F20"/>
-    <mergeCell ref="F21:F27"/>
-    <mergeCell ref="D14:E20"/>
-    <mergeCell ref="D21:E27"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D4:E13"/>
@@ -4530,6 +4524,12 @@
     <mergeCell ref="H12:L12"/>
     <mergeCell ref="H13:L13"/>
     <mergeCell ref="F10:F11"/>
+    <mergeCell ref="H10:L10"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="F14:F20"/>
+    <mergeCell ref="F21:F27"/>
+    <mergeCell ref="D14:E20"/>
+    <mergeCell ref="D21:E27"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:L27">
     <cfRule type="colorScale" priority="55">
@@ -4552,8 +4552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F339B4-372A-B44E-B41D-D416A194057A}">
   <dimension ref="B1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -4572,24 +4572,24 @@
     <row r="1" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B2" s="53"/>
-      <c r="D2" s="113" t="s">
+      <c r="D2" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="114" t="s">
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="102" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="114"/>
-      <c r="J2" s="115"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="103"/>
     </row>
     <row r="3" spans="2:14" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="53"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="118"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="106"/>
       <c r="H3" s="60" t="s">
         <v>50</v>
       </c>
@@ -4604,11 +4604,11 @@
       <c r="B4" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="119" t="s">
+      <c r="D4" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="120"/>
-      <c r="F4" s="122" t="s">
+      <c r="E4" s="108"/>
+      <c r="F4" s="112" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="63" t="s">
@@ -4617,32 +4617,32 @@
       <c r="H4" s="125">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="107"/>
-      <c r="J4" s="108"/>
+      <c r="I4" s="118"/>
+      <c r="J4" s="119"/>
     </row>
     <row r="5" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="103"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="112"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="113"/>
       <c r="G5" s="64" t="s">
         <v>36</v>
       </c>
       <c r="H5" s="126">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="123"/>
-      <c r="J5" s="124"/>
+      <c r="I5" s="116"/>
+      <c r="J5" s="117"/>
     </row>
     <row r="6" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="103"/>
-      <c r="E6" s="120"/>
-      <c r="F6" s="122" t="s">
+      <c r="D6" s="109"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="112" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="22" t="s">
@@ -4651,28 +4651,28 @@
       <c r="H6" s="125">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="107"/>
-      <c r="J6" s="108"/>
+      <c r="I6" s="118"/>
+      <c r="J6" s="119"/>
     </row>
     <row r="7" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="52"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="120"/>
-      <c r="F7" s="112"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="113"/>
       <c r="G7" s="64" t="s">
         <v>38</v>
       </c>
       <c r="H7" s="126">
         <v>0.85199999999999998</v>
       </c>
-      <c r="I7" s="123"/>
-      <c r="J7" s="124"/>
+      <c r="I7" s="116"/>
+      <c r="J7" s="117"/>
     </row>
     <row r="8" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="53"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="120"/>
-      <c r="F8" s="122" t="s">
+      <c r="D8" s="109"/>
+      <c r="E8" s="108"/>
+      <c r="F8" s="112" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="22" t="s">
@@ -4681,27 +4681,27 @@
       <c r="H8" s="125">
         <v>0.65400000000000003</v>
       </c>
-      <c r="I8" s="107"/>
-      <c r="J8" s="108"/>
+      <c r="I8" s="118"/>
+      <c r="J8" s="119"/>
     </row>
     <row r="9" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="53"/>
-      <c r="D9" s="103"/>
-      <c r="E9" s="120"/>
-      <c r="F9" s="112"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="108"/>
+      <c r="F9" s="113"/>
       <c r="G9" s="64" t="s">
         <v>40</v>
       </c>
       <c r="H9" s="126">
         <v>0.753</v>
       </c>
-      <c r="I9" s="123"/>
-      <c r="J9" s="124"/>
+      <c r="I9" s="116"/>
+      <c r="J9" s="117"/>
     </row>
     <row r="10" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="103"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="122" t="s">
+      <c r="D10" s="109"/>
+      <c r="E10" s="108"/>
+      <c r="F10" s="112" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="65" t="s">
@@ -4710,26 +4710,26 @@
       <c r="H10" s="125">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I10" s="107"/>
-      <c r="J10" s="108"/>
+      <c r="I10" s="118"/>
+      <c r="J10" s="119"/>
     </row>
     <row r="11" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="103"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="112"/>
+      <c r="D11" s="109"/>
+      <c r="E11" s="108"/>
+      <c r="F11" s="113"/>
       <c r="G11" s="66" t="s">
         <v>42</v>
       </c>
       <c r="H11" s="126">
         <v>0.98699999999999999</v>
       </c>
-      <c r="I11" s="123"/>
-      <c r="J11" s="124"/>
+      <c r="I11" s="116"/>
+      <c r="J11" s="117"/>
     </row>
     <row r="12" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="103"/>
-      <c r="E12" s="120"/>
-      <c r="F12" s="122" t="s">
+      <c r="D12" s="109"/>
+      <c r="E12" s="108"/>
+      <c r="F12" s="112" t="s">
         <v>21</v>
       </c>
       <c r="G12" s="65" t="s">
@@ -4738,28 +4738,28 @@
       <c r="H12" s="125">
         <v>0.71499999999999997</v>
       </c>
-      <c r="I12" s="107"/>
-      <c r="J12" s="108"/>
+      <c r="I12" s="118"/>
+      <c r="J12" s="119"/>
     </row>
     <row r="13" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="105"/>
-      <c r="E13" s="121"/>
-      <c r="F13" s="111"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="120"/>
       <c r="G13" s="23" t="s">
         <v>44</v>
       </c>
       <c r="H13" s="126">
         <v>0.99</v>
       </c>
-      <c r="I13" s="123"/>
-      <c r="J13" s="124"/>
+      <c r="I13" s="116"/>
+      <c r="J13" s="117"/>
     </row>
     <row r="14" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" s="127" t="s">
         <v>60</v>
       </c>
       <c r="E14" s="128"/>
-      <c r="F14" s="102"/>
+      <c r="F14" s="122"/>
       <c r="G14" s="21" t="s">
         <v>6</v>
       </c>
@@ -4773,9 +4773,9 @@
       <c r="N14" s="5"/>
     </row>
     <row r="15" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="103"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="104"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="108"/>
+      <c r="F15" s="123"/>
       <c r="G15" s="1" t="s">
         <v>54</v>
       </c>
@@ -4789,9 +4789,9 @@
       <c r="N15" s="5"/>
     </row>
     <row r="16" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="105"/>
-      <c r="E16" s="121"/>
-      <c r="F16" s="106"/>
+      <c r="D16" s="110"/>
+      <c r="E16" s="111"/>
+      <c r="F16" s="124"/>
       <c r="G16" s="15" t="s">
         <v>55</v>
       </c>
@@ -4829,15 +4829,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="D14:F16"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="H13:J13"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="D4:E13"/>
@@ -4848,19 +4839,16 @@
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="F8:F9"/>
+    <mergeCell ref="D14:F16"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H13:J13"/>
   </mergeCells>
-  <conditionalFormatting sqref="H4:J16">
-    <cfRule type="colorScale" priority="64">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-        <color theme="6" tint="-0.249977111117893"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H19:I20">
     <cfRule type="colorScale" priority="2">
       <colorScale>
@@ -4885,6 +4873,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H4:J16">
+    <cfRule type="colorScale" priority="64">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color theme="6" tint="-0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -4892,10 +4892,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D718D1-05D9-2146-B7ED-D601D310FD08}">
-  <dimension ref="B1:AB22"/>
+  <dimension ref="B1:AB27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -4926,28 +4926,28 @@
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="2:28" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="133"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="131" t="s">
+      <c r="C2" s="136"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="137" t="s">
+      <c r="F2" s="140" t="s">
         <v>57</v>
       </c>
-      <c r="G2" s="130"/>
-      <c r="H2" s="137" t="s">
+      <c r="G2" s="133"/>
+      <c r="H2" s="140" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="130"/>
-      <c r="J2" s="129" t="s">
+      <c r="I2" s="133"/>
+      <c r="J2" s="132" t="s">
         <v>59</v>
       </c>
-      <c r="K2" s="130"/>
+      <c r="K2" s="133"/>
     </row>
     <row r="3" spans="2:28" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="135"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="132"/>
+      <c r="C3" s="138"/>
+      <c r="D3" s="139"/>
+      <c r="E3" s="135"/>
       <c r="F3" s="70" t="s">
         <v>54</v>
       </c>
@@ -4968,10 +4968,10 @@
       </c>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="C4" s="133" t="s">
+      <c r="C4" s="136" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="134"/>
+      <c r="D4" s="137"/>
       <c r="E4" s="78">
         <v>0.501</v>
       </c>
@@ -4995,10 +4995,10 @@
       </c>
     </row>
     <row r="5" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="90" t="s">
+      <c r="C5" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="138"/>
+      <c r="D5" s="131"/>
       <c r="E5" s="74">
         <v>0.65400000000000003</v>
       </c>
@@ -5020,12 +5020,16 @@
       <c r="K5" s="23">
         <v>0.99199999999999999</v>
       </c>
+      <c r="O5" s="1">
+        <f>AVERAGE(I4:I7)</f>
+        <v>0.9484999999999999</v>
+      </c>
     </row>
     <row r="6" spans="2:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="90" t="s">
+      <c r="C6" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="138"/>
+      <c r="D6" s="131"/>
       <c r="E6" s="74">
         <v>0.73499999999999999</v>
       </c>
@@ -5047,12 +5051,16 @@
       <c r="K6" s="23">
         <v>0.995</v>
       </c>
+      <c r="O6" s="5">
+        <f>AVERAGE(I8:I10)</f>
+        <v>0.98366666666666669</v>
+      </c>
     </row>
     <row r="7" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="90" t="s">
+      <c r="C7" s="87" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="138"/>
+      <c r="D7" s="131"/>
       <c r="E7" s="75">
         <v>0.71499999999999997</v>
       </c>
@@ -5076,10 +5084,10 @@
       </c>
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="C8" s="90" t="s">
+      <c r="C8" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="138"/>
+      <c r="D8" s="131"/>
       <c r="E8" s="74">
         <v>0.94799999999999995</v>
       </c>
@@ -5103,10 +5111,10 @@
       </c>
     </row>
     <row r="9" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="90" t="s">
+      <c r="C9" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="138"/>
+      <c r="D9" s="131"/>
       <c r="E9" s="74">
         <v>0.98699999999999999</v>
       </c>
@@ -5143,10 +5151,10 @@
       <c r="AB9" s="10"/>
     </row>
     <row r="10" spans="2:28" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="139" t="s">
+      <c r="C10" s="129" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="140"/>
+      <c r="D10" s="130"/>
       <c r="E10" s="76">
         <v>0.99</v>
       </c>
@@ -5198,20 +5206,11 @@
       <c r="AB11" s="10"/>
     </row>
     <row r="12" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="G12" s="5">
-        <f>(G4-$E4)/$E4</f>
-        <v>0.88822355289421151</v>
-      </c>
+      <c r="G12" s="5"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="5">
-        <f>(I4-$E4)/$E4</f>
-        <v>0.88223552894211565</v>
-      </c>
+      <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="5">
-        <f>(K4-$E4)/$E4</f>
-        <v>0.96407185628742509</v>
-      </c>
+      <c r="K12" s="5"/>
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
       <c r="R12" s="10"/>
@@ -5227,20 +5226,11 @@
       <c r="AB12" s="10"/>
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="G13" s="5">
-        <f>(G5-$E5)/$E5</f>
-        <v>0.44495412844036686</v>
-      </c>
+      <c r="G13" s="5"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="5">
-        <f>(I5-$E5)/$E5</f>
-        <v>0.46330275229357787</v>
-      </c>
+      <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="5">
-        <f>(K5-$E5)/$E5</f>
-        <v>0.51681957186544336</v>
-      </c>
+      <c r="K13" s="5"/>
       <c r="P13" s="10"/>
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
@@ -5256,20 +5246,11 @@
       <c r="AB13" s="10"/>
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="G14" s="5">
-        <f t="shared" ref="G14:I18" si="0">(G6-$E6)/$E6</f>
-        <v>0.30204081632653057</v>
-      </c>
+      <c r="G14" s="5"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="5">
-        <f t="shared" si="0"/>
-        <v>0.29251700680272102</v>
-      </c>
+      <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="5">
-        <f t="shared" ref="K14" si="1">(K6-$E6)/$E6</f>
-        <v>0.35374149659863946</v>
-      </c>
+      <c r="K14" s="5"/>
       <c r="P14" s="10"/>
       <c r="Q14" s="10"/>
       <c r="R14" s="10"/>
@@ -5285,20 +5266,11 @@
       <c r="AB14" s="10"/>
     </row>
     <row r="15" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="G15" s="5">
-        <f t="shared" si="0"/>
-        <v>0.34405594405594409</v>
-      </c>
+      <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="5">
-        <f t="shared" si="0"/>
-        <v>0.32027972027972029</v>
-      </c>
+      <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="5">
-        <f t="shared" ref="K15" si="2">(K7-$E7)/$E7</f>
-        <v>0.38321678321678326</v>
-      </c>
+      <c r="K15" s="5"/>
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
       <c r="R15" s="10"/>
@@ -5314,20 +5286,11 @@
       <c r="AB15" s="10"/>
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="G16" s="5">
-        <f t="shared" si="0"/>
-        <v>1.8987341772151917E-2</v>
-      </c>
+      <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="5">
-        <f t="shared" si="0"/>
-        <v>2.7426160337552768E-2</v>
-      </c>
+      <c r="I16" s="5"/>
       <c r="J16" s="5"/>
-      <c r="K16" s="5">
-        <f t="shared" ref="K16" si="3">(K8-$E8)/$E8</f>
-        <v>2.9535864978902981E-2</v>
-      </c>
+      <c r="K16" s="5"/>
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
       <c r="R16" s="10"/>
@@ -5347,36 +5310,18 @@
       <c r="D17" s="42"/>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
-      <c r="G17" s="5">
-        <f t="shared" si="0"/>
-        <v>-3.5460992907801449E-2</v>
-      </c>
+      <c r="G17" s="5"/>
       <c r="H17" s="5"/>
-      <c r="I17" s="5">
-        <f t="shared" si="0"/>
-        <v>1.0131712259371843E-3</v>
-      </c>
+      <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="5">
-        <f t="shared" ref="K17" si="4">(K9-$E9)/$E9</f>
-        <v>3.0395136778115527E-3</v>
-      </c>
+      <c r="K17" s="5"/>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C18" s="42"/>
       <c r="D18" s="42"/>
-      <c r="G18" s="5">
-        <f t="shared" si="0"/>
-        <v>-3.5353535353535387E-2</v>
-      </c>
-      <c r="I18" s="5">
-        <f t="shared" si="0"/>
-        <v>-1.010101010101011E-3</v>
-      </c>
-      <c r="K18" s="5">
-        <f t="shared" ref="K18" si="5">(K10-$E10)/$E10</f>
-        <v>4.0404040404040439E-3</v>
-      </c>
+      <c r="G18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="K18" s="5"/>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C19" s="42"/>
@@ -5386,34 +5331,16 @@
       <c r="I19" s="42"/>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="G20" s="5">
-        <f>AVERAGE(G13:G15)</f>
-        <v>0.36368362960761386</v>
-      </c>
-      <c r="I20" s="5">
-        <f>AVERAGE(I13:I15)</f>
-        <v>0.3586998264586731</v>
-      </c>
-      <c r="K20" s="5">
-        <f>AVERAGE(K13:K15)</f>
-        <v>0.41792595056028864</v>
-      </c>
+      <c r="G20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="K20" s="5"/>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C21" s="42"/>
       <c r="D21" s="42"/>
-      <c r="G21" s="5">
-        <f>AVERAGE(G16:G18)</f>
-        <v>-1.7275728829728308E-2</v>
-      </c>
-      <c r="I21" s="5">
-        <f>AVERAGE(I16:I18)</f>
-        <v>9.1430768511296476E-3</v>
-      </c>
-      <c r="K21" s="5">
-        <f>AVERAGE(K16:K18)</f>
-        <v>1.2205260899039526E-2</v>
-      </c>
+      <c r="G21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="K21" s="5"/>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C22" s="42"/>
@@ -5422,20 +5349,23 @@
       <c r="G22" s="42"/>
       <c r="I22" s="42"/>
     </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="G27" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="C2:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="C2:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:K7 E10:K10">
     <cfRule type="colorScale" priority="5">

</xml_diff>